<commit_message>
Add fine arts > artists' books collection to location facet
DISCOVERYACCESS-4992
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frances\Documents\GitHub\da-solr-availability\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5E7CFC-88A1-492A-A4D4-1347F76A065E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="216">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -662,12 +661,18 @@
   </si>
   <si>
     <t>Kroch Library Rare &amp; Manuscripts &gt; Technical Services</t>
+  </si>
+  <si>
+    <t>Artist</t>
+  </si>
+  <si>
+    <t>Fine Arts Library &gt; Artists' Books</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1502,11 +1507,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E111"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1651,80 +1656,83 @@
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C16" t="s">
+        <v>214</v>
+      </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E23" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E24" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E25" t="s">
         <v>42</v>
@@ -1732,7 +1740,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E26" t="s">
         <v>42</v>
@@ -1740,15 +1748,15 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E27" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E28" t="s">
         <v>46</v>
@@ -1756,144 +1764,141 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E29" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B32" t="s">
-        <v>147</v>
+        <v>52</v>
       </c>
       <c r="E32" t="s">
-        <v>213</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>54</v>
+        <v>212</v>
+      </c>
+      <c r="B33" t="s">
+        <v>147</v>
       </c>
       <c r="E33" t="s">
-        <v>55</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E35" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E38" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E39" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E41" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E42" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E44" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" t="s">
-        <v>201</v>
+        <v>75</v>
       </c>
       <c r="E45" t="s">
-        <v>202</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1901,143 +1906,146 @@
         <v>77</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>201</v>
       </c>
       <c r="E46" t="s">
-        <v>79</v>
+        <v>202</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="C47" t="s">
+        <v>78</v>
+      </c>
       <c r="E47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E48" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E49" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E50" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E51" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E52" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E53" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E54" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E55" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E56" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E57" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E58" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E59" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E60" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E61" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E62" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E63" t="s">
         <v>110</v>
@@ -2045,252 +2053,249 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E64" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E65" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C66" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E66" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>116</v>
       </c>
+      <c r="C67" t="s">
+        <v>117</v>
+      </c>
       <c r="E67" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E68" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E69" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E70" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E71" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E72" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E73" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E74" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E75" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E76" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E77" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E78" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E79" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E80" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B81" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E81" t="s">
-        <v>211</v>
+        <v>145</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B82" t="s">
         <v>147</v>
       </c>
       <c r="E82" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>146</v>
+        <v>206</v>
       </c>
       <c r="B83" t="s">
         <v>147</v>
       </c>
       <c r="E83" t="s">
-        <v>148</v>
+        <v>207</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>208</v>
+        <v>146</v>
       </c>
       <c r="B84" t="s">
         <v>147</v>
       </c>
       <c r="E84" t="s">
-        <v>207</v>
+        <v>148</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>149</v>
+        <v>208</v>
+      </c>
+      <c r="B85" t="s">
+        <v>147</v>
       </c>
       <c r="E85" t="s">
-        <v>150</v>
+        <v>207</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E86" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E87" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E88" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E89" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E90" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E91" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C92" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E92" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2298,10 +2303,10 @@
         <v>163</v>
       </c>
       <c r="C93" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E93" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2309,10 +2314,10 @@
         <v>163</v>
       </c>
       <c r="C94" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E94" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2320,10 +2325,10 @@
         <v>163</v>
       </c>
       <c r="C95" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E95" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2331,120 +2336,120 @@
         <v>163</v>
       </c>
       <c r="C96" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E96" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>163</v>
       </c>
+      <c r="C97" t="s">
+        <v>172</v>
+      </c>
       <c r="E97" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="E98" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E99" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E100" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E101" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E102" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E103" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E104" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E105" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B106" t="s">
-        <v>147</v>
+        <v>189</v>
       </c>
       <c r="E106" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B107" t="s">
         <v>147</v>
       </c>
       <c r="E107" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B108" t="s">
         <v>147</v>
       </c>
       <c r="E108" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B109" t="s">
         <v>147</v>
@@ -2454,8 +2459,8 @@
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>205</v>
+      <c r="A110" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="B110" t="s">
         <v>147</v>
@@ -2466,12 +2471,23 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B111" t="s">
         <v>147</v>
       </c>
       <c r="E111" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>209</v>
+      </c>
+      <c r="B112" t="s">
+        <v>147</v>
+      </c>
+      <c r="E112" t="s">
         <v>196</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Associate Artists' Books subcollection with fine arts reference, not main coll.
DISCOVERYACCESS-4992
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -1511,7 +1511,7 @@
   <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,19 +1656,19 @@
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C16" t="s">
-        <v>214</v>
-      </c>
       <c r="E16" t="s">
-        <v>215</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>214</v>
       </c>
       <c r="E17" t="s">
-        <v>27</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Change display name of fine arts library back to Rand for location facet
DISCOVERYACCESS-4992
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -2,19 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookPr checkCompatibility="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27690" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -99,9 +95,6 @@
     <t>Fine Arts Library &gt; Circulation</t>
   </si>
   <si>
-    <t>Fine Arts Library (B56 Sibley Hall)</t>
-  </si>
-  <si>
     <t>Fine Arts Library &gt; Main Collection</t>
   </si>
   <si>
@@ -667,6 +660,9 @@
   </si>
   <si>
     <t>Fine Arts Library &gt; Artists' Books</t>
+  </si>
+  <si>
+    <t>Fine Arts Library (Rand Hall)</t>
   </si>
 </sst>
 </file>
@@ -1511,7 +1507,7 @@
   <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,7 +1521,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1536,10 +1532,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -1579,10 +1575,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>202</v>
+      </c>
+      <c r="E7" t="s">
         <v>203</v>
-      </c>
-      <c r="E7" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1654,841 +1650,841 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E16" t="s">
         <v>26</v>
-      </c>
-      <c r="E16" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
+        <v>213</v>
+      </c>
+      <c r="E17" t="s">
         <v>214</v>
-      </c>
-      <c r="E17" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" t="s">
         <v>28</v>
-      </c>
-      <c r="E18" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" t="s">
         <v>30</v>
-      </c>
-      <c r="E19" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
         <v>32</v>
-      </c>
-      <c r="E20" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
         <v>34</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
         <v>35</v>
-      </c>
-      <c r="E21" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" t="s">
         <v>38</v>
-      </c>
-      <c r="E23" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" t="s">
         <v>41</v>
-      </c>
-      <c r="E25" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" t="s">
         <v>45</v>
-      </c>
-      <c r="E28" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" t="s">
         <v>48</v>
-      </c>
-      <c r="E30" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" t="s">
         <v>50</v>
-      </c>
-      <c r="E31" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" t="s">
         <v>52</v>
-      </c>
-      <c r="E32" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B33" t="s">
+        <v>146</v>
+      </c>
+      <c r="E33" t="s">
         <v>212</v>
-      </c>
-      <c r="B33" t="s">
-        <v>147</v>
-      </c>
-      <c r="E33" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" t="s">
         <v>54</v>
-      </c>
-      <c r="E34" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" t="s">
         <v>56</v>
-      </c>
-      <c r="E35" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" t="s">
         <v>58</v>
-      </c>
-      <c r="E36" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" t="s">
         <v>60</v>
-      </c>
-      <c r="E37" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" t="s">
         <v>62</v>
-      </c>
-      <c r="E38" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" t="s">
         <v>64</v>
-      </c>
-      <c r="E39" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" t="s">
         <v>66</v>
-      </c>
-      <c r="E40" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E41" t="s">
         <v>68</v>
-      </c>
-      <c r="E41" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E42" t="s">
         <v>70</v>
-      </c>
-      <c r="E42" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E43" t="s">
         <v>72</v>
-      </c>
-      <c r="E43" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E45" t="s">
         <v>75</v>
-      </c>
-      <c r="E45" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C46" t="s">
+        <v>200</v>
+      </c>
+      <c r="E46" t="s">
         <v>201</v>
-      </c>
-      <c r="E46" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" t="s">
         <v>77</v>
       </c>
-      <c r="C47" t="s">
+      <c r="E47" t="s">
         <v>78</v>
-      </c>
-      <c r="E47" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E49" t="s">
         <v>81</v>
-      </c>
-      <c r="E49" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E50" t="s">
         <v>83</v>
-      </c>
-      <c r="E50" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E51" t="s">
         <v>85</v>
-      </c>
-      <c r="E51" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" t="s">
         <v>87</v>
-      </c>
-      <c r="E52" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E53" t="s">
         <v>89</v>
-      </c>
-      <c r="E53" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E54" t="s">
         <v>91</v>
-      </c>
-      <c r="E54" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E55" t="s">
         <v>93</v>
-      </c>
-      <c r="E55" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E56" t="s">
         <v>95</v>
-      </c>
-      <c r="E56" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E57" t="s">
         <v>97</v>
-      </c>
-      <c r="E57" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E58" t="s">
         <v>99</v>
-      </c>
-      <c r="E58" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E59" t="s">
         <v>101</v>
-      </c>
-      <c r="E59" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E60" t="s">
         <v>103</v>
-      </c>
-      <c r="E60" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E61" t="s">
         <v>105</v>
-      </c>
-      <c r="E61" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E62" t="s">
         <v>107</v>
-      </c>
-      <c r="E62" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E63" t="s">
         <v>109</v>
-      </c>
-      <c r="E63" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E64" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E65" t="s">
         <v>112</v>
-      </c>
-      <c r="E65" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E66" t="s">
         <v>114</v>
-      </c>
-      <c r="E66" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C67" t="s">
         <v>116</v>
       </c>
-      <c r="C67" t="s">
+      <c r="E67" t="s">
         <v>117</v>
-      </c>
-      <c r="E67" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E68" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E69" t="s">
         <v>120</v>
-      </c>
-      <c r="E69" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E70" t="s">
         <v>122</v>
-      </c>
-      <c r="E70" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E71" t="s">
         <v>124</v>
-      </c>
-      <c r="E71" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E72" t="s">
         <v>126</v>
-      </c>
-      <c r="E72" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E73" t="s">
         <v>128</v>
-      </c>
-      <c r="E73" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E74" t="s">
         <v>130</v>
-      </c>
-      <c r="E74" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E75" t="s">
         <v>132</v>
-      </c>
-      <c r="E75" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E76" t="s">
         <v>134</v>
-      </c>
-      <c r="E76" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E77" t="s">
         <v>136</v>
-      </c>
-      <c r="E77" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E78" t="s">
         <v>138</v>
-      </c>
-      <c r="E78" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E79" t="s">
         <v>140</v>
-      </c>
-      <c r="E79" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E80" t="s">
         <v>142</v>
-      </c>
-      <c r="E80" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E81" t="s">
         <v>144</v>
-      </c>
-      <c r="E81" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B82" t="s">
+        <v>146</v>
+      </c>
+      <c r="E82" t="s">
         <v>210</v>
-      </c>
-      <c r="B82" t="s">
-        <v>147</v>
-      </c>
-      <c r="E82" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B83" t="s">
+        <v>146</v>
+      </c>
+      <c r="E83" t="s">
         <v>206</v>
-      </c>
-      <c r="B83" t="s">
-        <v>147</v>
-      </c>
-      <c r="E83" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B84" t="s">
         <v>146</v>
       </c>
-      <c r="B84" t="s">
+      <c r="E84" t="s">
         <v>147</v>
-      </c>
-      <c r="E84" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B85" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E85" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E86" t="s">
         <v>149</v>
-      </c>
-      <c r="E86" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E87" t="s">
         <v>151</v>
-      </c>
-      <c r="E87" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E88" t="s">
         <v>153</v>
-      </c>
-      <c r="E88" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E89" t="s">
         <v>155</v>
-      </c>
-      <c r="E89" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E90" t="s">
         <v>157</v>
-      </c>
-      <c r="E90" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E91" t="s">
         <v>159</v>
-      </c>
-      <c r="E91" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E92" t="s">
         <v>161</v>
-      </c>
-      <c r="E92" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C93" t="s">
         <v>163</v>
       </c>
-      <c r="C93" t="s">
+      <c r="E93" t="s">
         <v>164</v>
-      </c>
-      <c r="E93" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C94" t="s">
+        <v>165</v>
+      </c>
+      <c r="E94" t="s">
         <v>166</v>
-      </c>
-      <c r="E94" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C95" t="s">
+        <v>167</v>
+      </c>
+      <c r="E95" t="s">
         <v>168</v>
-      </c>
-      <c r="E95" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C96" t="s">
+        <v>169</v>
+      </c>
+      <c r="E96" t="s">
         <v>170</v>
-      </c>
-      <c r="E96" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C97" t="s">
+        <v>171</v>
+      </c>
+      <c r="E97" t="s">
         <v>172</v>
-      </c>
-      <c r="E97" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E98" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E99" t="s">
         <v>175</v>
-      </c>
-      <c r="E99" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E100" t="s">
         <v>177</v>
-      </c>
-      <c r="E100" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E101" t="s">
         <v>179</v>
-      </c>
-      <c r="E101" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E102" t="s">
         <v>181</v>
-      </c>
-      <c r="E102" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E103" t="s">
         <v>183</v>
-      </c>
-      <c r="E103" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E104" t="s">
         <v>185</v>
-      </c>
-      <c r="E104" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E105" t="s">
         <v>187</v>
-      </c>
-      <c r="E105" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E106" t="s">
         <v>189</v>
-      </c>
-      <c r="E106" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B107" t="s">
+        <v>146</v>
+      </c>
+      <c r="E107" t="s">
         <v>191</v>
-      </c>
-      <c r="B107" t="s">
-        <v>147</v>
-      </c>
-      <c r="E107" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B108" t="s">
+        <v>146</v>
+      </c>
+      <c r="E108" t="s">
         <v>193</v>
-      </c>
-      <c r="B108" t="s">
-        <v>147</v>
-      </c>
-      <c r="E108" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B109" t="s">
+        <v>146</v>
+      </c>
+      <c r="E109" t="s">
         <v>195</v>
-      </c>
-      <c r="B109" t="s">
-        <v>147</v>
-      </c>
-      <c r="E109" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B110" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E110" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B111" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E111" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B112" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E112" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
apply location changes to facet
apply new mann special collections location, and music library location name
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr checkCompatibility="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27690" windowHeight="8205"/>
   </bookViews>
@@ -10,12 +15,11 @@
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="218">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -663,6 +667,12 @@
   </si>
   <si>
     <t>Fine Arts Library (Rand Hall)</t>
+  </si>
+  <si>
+    <t>Music Library (Lincoln Hall)</t>
+  </si>
+  <si>
+    <t>Mann Special Collections (Request in advance)</t>
   </si>
 </sst>
 </file>
@@ -1504,10 +1514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E112"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1969,267 +1979,261 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>90</v>
+        <v>217</v>
       </c>
       <c r="E54" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E55" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E56" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E57" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E58" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E59" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E60" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>104</v>
+        <v>216</v>
       </c>
       <c r="E61" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E62" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E63" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E64" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E65" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E66" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C67" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E67" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E68" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
+      </c>
+      <c r="C69" t="s">
+        <v>116</v>
       </c>
       <c r="E69" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E70" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E71" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E72" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E73" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E74" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E75" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E76" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E77" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E78" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E79" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E80" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E81" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B82" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E82" t="s">
-        <v>210</v>
+        <v>142</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B83" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E83" t="s">
-        <v>206</v>
+        <v>144</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>145</v>
+        <v>209</v>
       </c>
       <c r="B84" t="s">
         <v>146</v>
       </c>
       <c r="E84" t="s">
-        <v>147</v>
+        <v>210</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B85" t="s">
         <v>146</v>
@@ -2240,80 +2244,80 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
+      </c>
+      <c r="B86" t="s">
+        <v>146</v>
       </c>
       <c r="E86" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>150</v>
+        <v>207</v>
+      </c>
+      <c r="B87" t="s">
+        <v>146</v>
       </c>
       <c r="E87" t="s">
-        <v>151</v>
+        <v>206</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E88" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E89" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E90" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E91" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E92" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C93" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E93" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C94" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E94" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2321,10 +2325,10 @@
         <v>162</v>
       </c>
       <c r="C95" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E95" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2332,10 +2336,10 @@
         <v>162</v>
       </c>
       <c r="C96" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E96" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2343,131 +2347,131 @@
         <v>162</v>
       </c>
       <c r="C97" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E97" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="C98" t="s">
+        <v>169</v>
+      </c>
       <c r="E98" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
+      </c>
+      <c r="C99" t="s">
+        <v>171</v>
       </c>
       <c r="E99" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="E100" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E101" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E102" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E103" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E104" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E105" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E106" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B107" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="E107" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B108" t="s">
-        <v>146</v>
+        <v>188</v>
       </c>
       <c r="E108" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B109" t="s">
         <v>146</v>
       </c>
       <c r="E109" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B110" t="s">
         <v>146</v>
       </c>
       <c r="E110" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>204</v>
+      <c r="A111" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="B111" t="s">
         <v>146</v>
@@ -2477,13 +2481,35 @@
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>208</v>
+      <c r="A112" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="B112" t="s">
         <v>146</v>
       </c>
       <c r="E112" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>204</v>
+      </c>
+      <c r="B113" t="s">
+        <v>146</v>
+      </c>
+      <c r="E113" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>208</v>
+      </c>
+      <c r="B114" t="s">
+        <v>146</v>
+      </c>
+      <c r="E114" t="s">
         <v>195</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fine Arts Reserve location mapping updates
I'm putting both the regular and permanent reserve titles in the same "Fine Arts Library > Reserve" facet location until and unless I hear that they should be split up.
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="220">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -673,6 +673,12 @@
   </si>
   <si>
     <t>Mann Special Collections (Request in advance)</t>
+  </si>
+  <si>
+    <t>Fine Arts Library Permanent Reserve</t>
+  </si>
+  <si>
+    <t>Fine Arts Course Reserve (Ask at Circulation)</t>
   </si>
 </sst>
 </file>
@@ -1514,10 +1520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1687,7 +1693,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>218</v>
       </c>
       <c r="E19" t="s">
         <v>30</v>
@@ -1695,66 +1701,66 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>219</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E25" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E26" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E27" t="s">
         <v>41</v>
@@ -1762,500 +1768,494 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E28" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E29" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E30" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E31" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E32" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B33" t="s">
-        <v>146</v>
+        <v>49</v>
       </c>
       <c r="E33" t="s">
-        <v>212</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>55</v>
+        <v>211</v>
+      </c>
+      <c r="B35" t="s">
+        <v>146</v>
       </c>
       <c r="E35" t="s">
-        <v>56</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E36" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E37" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E38" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E39" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E40" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E41" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E42" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E43" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E44" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E45" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" t="s">
-        <v>200</v>
+        <v>73</v>
       </c>
       <c r="E46" t="s">
-        <v>201</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C47" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E47" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="C48" t="s">
+        <v>200</v>
+      </c>
       <c r="E48" t="s">
-        <v>79</v>
+        <v>201</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
+      </c>
+      <c r="C49" t="s">
+        <v>77</v>
       </c>
       <c r="E49" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E50" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E51" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E52" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E53" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>217</v>
+        <v>86</v>
       </c>
       <c r="E54" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E55" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>92</v>
+        <v>217</v>
       </c>
       <c r="E56" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E57" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E58" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E59" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E60" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>216</v>
+        <v>98</v>
       </c>
       <c r="E61" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E62" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>104</v>
+        <v>216</v>
       </c>
       <c r="E63" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E64" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E65" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E66" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E67" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E68" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C69" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E69" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E70" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
+      </c>
+      <c r="C71" t="s">
+        <v>116</v>
       </c>
       <c r="E71" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E72" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E73" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E74" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E75" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E76" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E77" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E78" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E79" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E80" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E81" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E82" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E83" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B84" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E84" t="s">
-        <v>210</v>
+        <v>142</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B85" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E85" t="s">
-        <v>206</v>
+        <v>144</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>145</v>
+        <v>209</v>
       </c>
       <c r="B86" t="s">
         <v>146</v>
       </c>
       <c r="E86" t="s">
-        <v>147</v>
+        <v>210</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B87" t="s">
         <v>146</v>
@@ -2266,80 +2266,80 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
+      </c>
+      <c r="B88" t="s">
+        <v>146</v>
       </c>
       <c r="E88" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>150</v>
+        <v>207</v>
+      </c>
+      <c r="B89" t="s">
+        <v>146</v>
       </c>
       <c r="E89" t="s">
-        <v>151</v>
+        <v>206</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E90" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E91" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E92" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E93" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E94" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C95" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E95" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C96" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E96" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2347,10 +2347,10 @@
         <v>162</v>
       </c>
       <c r="C97" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E97" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2358,10 +2358,10 @@
         <v>162</v>
       </c>
       <c r="C98" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E98" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2369,131 +2369,131 @@
         <v>162</v>
       </c>
       <c r="C99" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E99" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="C100" t="s">
+        <v>169</v>
+      </c>
       <c r="E100" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
+      </c>
+      <c r="C101" t="s">
+        <v>171</v>
       </c>
       <c r="E101" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="E102" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E103" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E104" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E105" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E106" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E107" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E108" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B109" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="E109" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B110" t="s">
-        <v>146</v>
+        <v>188</v>
       </c>
       <c r="E110" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B111" t="s">
         <v>146</v>
       </c>
       <c r="E111" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B112" t="s">
         <v>146</v>
       </c>
       <c r="E112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>204</v>
+      <c r="A113" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="B113" t="s">
         <v>146</v>
@@ -2503,13 +2503,35 @@
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>208</v>
+      <c r="A114" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="B114" t="s">
         <v>146</v>
       </c>
       <c r="E114" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>204</v>
+      </c>
+      <c r="B115" t="s">
+        <v>146</v>
+      </c>
+      <c r="E115" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>208</v>
+      </c>
+      <c r="B116" t="s">
+        <v>146</v>
+      </c>
+      <c r="E116" t="s">
         <v>195</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update location facet for vet,core
DISCOVERYACCESS-5975
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -567,12 +567,6 @@
     <t>Veterinary Library &gt; Main Collection</t>
   </si>
   <si>
-    <t>Veterinary Library Core Resource (Non-Circulating)</t>
-  </si>
-  <si>
-    <t>Veterinary Library &gt; Core Resources</t>
-  </si>
-  <si>
     <t>Veterinary Library Rare Books (Non-Circulating)</t>
   </si>
   <si>
@@ -679,6 +673,12 @@
   </si>
   <si>
     <t>Fine Arts Course Reserve (Ask at Circulation)</t>
+  </si>
+  <si>
+    <t>Veterinary Library Core Resource (5 hour loan)</t>
+  </si>
+  <si>
+    <t>Veterinary Library &gt; Core Textbooks</t>
   </si>
 </sst>
 </file>
@@ -1522,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1537,7 +1537,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1548,10 +1548,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -1591,10 +1591,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1666,7 +1666,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E16" t="s">
         <v>26</v>
@@ -1677,10 +1677,10 @@
         <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E17" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1693,7 +1693,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E19" t="s">
         <v>30</v>
@@ -1701,7 +1701,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E20" t="s">
         <v>30</v>
@@ -1824,13 +1824,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B35" t="s">
         <v>146</v>
       </c>
       <c r="E35" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1934,10 +1934,10 @@
         <v>76</v>
       </c>
       <c r="C48" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E48" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2001,7 +2001,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E56" t="s">
         <v>89</v>
@@ -2057,7 +2057,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E63" t="s">
         <v>103</v>
@@ -2244,24 +2244,24 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B86" t="s">
         <v>146</v>
       </c>
       <c r="E86" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B87" t="s">
         <v>146</v>
       </c>
       <c r="E87" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2277,13 +2277,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B89" t="s">
         <v>146</v>
       </c>
       <c r="E89" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2439,100 +2439,100 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>182</v>
+        <v>218</v>
       </c>
       <c r="E107" t="s">
-        <v>183</v>
+        <v>219</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E108" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E109" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E110" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B111" t="s">
         <v>146</v>
       </c>
       <c r="E111" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B112" t="s">
         <v>146</v>
       </c>
       <c r="E112" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B113" t="s">
         <v>146</v>
       </c>
       <c r="E113" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B114" t="s">
         <v>146</v>
       </c>
       <c r="E114" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B115" t="s">
         <v>146</v>
       </c>
       <c r="E115" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B116" t="s">
         <v>146</v>
       </c>
       <c r="E116" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Africana A/V to facet map
DISCOVERYACCESS-7324
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="222">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -679,6 +679,12 @@
   </si>
   <si>
     <t>Veterinary Library &gt; Core Textbooks</t>
+  </si>
+  <si>
+    <t>Africana A/V</t>
+  </si>
+  <si>
+    <t>Africana Library &gt; A/V</t>
   </si>
 </sst>
 </file>
@@ -1520,10 +1526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,110 +1604,110 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
+      <c r="A8" t="s">
+        <v>220</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>213</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E17" t="s">
-        <v>212</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C18" t="s">
+        <v>211</v>
+      </c>
       <c r="E18" t="s">
-        <v>28</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>216</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E20" t="s">
         <v>30</v>
@@ -1709,7 +1715,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>217</v>
       </c>
       <c r="E21" t="s">
         <v>30</v>
@@ -1717,58 +1723,58 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E26" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E27" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E28" t="s">
         <v>41</v>
@@ -1776,7 +1782,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E29" t="s">
         <v>41</v>
@@ -1784,15 +1790,15 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E30" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E31" t="s">
         <v>45</v>
@@ -1800,144 +1806,141 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E32" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E34" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B35" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="E35" t="s">
-        <v>210</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>53</v>
+        <v>209</v>
+      </c>
+      <c r="B36" t="s">
+        <v>146</v>
       </c>
       <c r="E36" t="s">
-        <v>54</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E38" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E40" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E41" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E42" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E43" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E45" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E47" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C48" t="s">
-        <v>198</v>
+        <v>74</v>
       </c>
       <c r="E48" t="s">
-        <v>199</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1945,63 +1948,66 @@
         <v>76</v>
       </c>
       <c r="C49" t="s">
-        <v>77</v>
+        <v>198</v>
       </c>
       <c r="E49" t="s">
-        <v>78</v>
+        <v>199</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="C50" t="s">
+        <v>77</v>
+      </c>
       <c r="E50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E51" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E52" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E53" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E54" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>215</v>
+        <v>88</v>
       </c>
       <c r="E56" t="s">
         <v>89</v>
@@ -2009,63 +2015,63 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>90</v>
+        <v>215</v>
       </c>
       <c r="E57" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E58" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E59" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E60" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E61" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E62" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>214</v>
+        <v>100</v>
       </c>
       <c r="E63" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>102</v>
+        <v>214</v>
       </c>
       <c r="E64" t="s">
         <v>103</v>
@@ -2073,31 +2079,31 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E65" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E66" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E67" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E68" t="s">
         <v>109</v>
@@ -2105,252 +2111,249 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E69" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E70" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C71" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E71" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="C72" t="s">
+        <v>116</v>
+      </c>
       <c r="E72" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E73" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E74" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E75" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E76" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E77" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E78" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E79" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E80" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E81" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E82" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E83" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E84" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E85" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B86" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E86" t="s">
-        <v>208</v>
+        <v>144</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B87" t="s">
         <v>146</v>
       </c>
       <c r="E87" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>145</v>
+        <v>203</v>
       </c>
       <c r="B88" t="s">
         <v>146</v>
       </c>
       <c r="E88" t="s">
-        <v>147</v>
+        <v>204</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>205</v>
+        <v>145</v>
       </c>
       <c r="B89" t="s">
         <v>146</v>
       </c>
       <c r="E89" t="s">
-        <v>204</v>
+        <v>147</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>148</v>
+        <v>205</v>
+      </c>
+      <c r="B90" t="s">
+        <v>146</v>
       </c>
       <c r="E90" t="s">
-        <v>149</v>
+        <v>204</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E91" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E92" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E93" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E94" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E95" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E96" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C97" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E97" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2358,10 +2361,10 @@
         <v>162</v>
       </c>
       <c r="C98" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E98" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2369,10 +2372,10 @@
         <v>162</v>
       </c>
       <c r="C99" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E99" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2380,10 +2383,10 @@
         <v>162</v>
       </c>
       <c r="C100" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E100" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2391,120 +2394,120 @@
         <v>162</v>
       </c>
       <c r="C101" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E101" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="C102" t="s">
+        <v>171</v>
+      </c>
       <c r="E102" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E103" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E104" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E105" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E106" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>218</v>
+        <v>180</v>
       </c>
       <c r="E107" t="s">
-        <v>219</v>
+        <v>181</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>182</v>
+        <v>218</v>
       </c>
       <c r="E108" t="s">
-        <v>183</v>
+        <v>219</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E109" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E110" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B111" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="E111" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B112" t="s">
         <v>146</v>
       </c>
       <c r="E112" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B113" t="s">
         <v>146</v>
       </c>
       <c r="E113" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B114" t="s">
         <v>146</v>
@@ -2514,8 +2517,8 @@
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>202</v>
+      <c r="A115" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="B115" t="s">
         <v>146</v>
@@ -2526,12 +2529,23 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B116" t="s">
         <v>146</v>
       </c>
       <c r="E116" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>206</v>
+      </c>
+      <c r="B117" t="s">
+        <v>146</v>
+      </c>
+      <c r="E117" t="s">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add location facet mapping for ILR Permanent Reserve
DISCOVERYACCESS-7417
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr checkCompatibility="1"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="223">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -685,6 +685,9 @@
   </si>
   <si>
     <t>Africana Library &gt; A/V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILR Library Permanent Reserve </t>
   </si>
 </sst>
 </file>
@@ -1526,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E117"/>
+  <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1758,7 +1761,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>222</v>
       </c>
       <c r="E26" t="s">
         <v>38</v>
@@ -1766,23 +1769,23 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E27" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E28" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E29" t="s">
         <v>41</v>
@@ -1790,7 +1793,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E30" t="s">
         <v>41</v>
@@ -1798,15 +1801,15 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E31" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E32" t="s">
         <v>45</v>
@@ -1814,144 +1817,141 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E33" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E34" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B36" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="E36" t="s">
-        <v>210</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>53</v>
+        <v>209</v>
+      </c>
+      <c r="B37" t="s">
+        <v>146</v>
       </c>
       <c r="E37" t="s">
-        <v>54</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E39" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E42" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E44" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E45" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E46" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C49" t="s">
-        <v>198</v>
+        <v>74</v>
       </c>
       <c r="E49" t="s">
-        <v>199</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1959,63 +1959,66 @@
         <v>76</v>
       </c>
       <c r="C50" t="s">
-        <v>77</v>
+        <v>198</v>
       </c>
       <c r="E50" t="s">
-        <v>78</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="C51" t="s">
+        <v>77</v>
+      </c>
       <c r="E51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E52" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E53" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E54" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E55" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E56" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>215</v>
+        <v>88</v>
       </c>
       <c r="E57" t="s">
         <v>89</v>
@@ -2023,63 +2026,63 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>90</v>
+        <v>215</v>
       </c>
       <c r="E58" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E59" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E60" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E61" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E62" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E63" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>214</v>
+        <v>100</v>
       </c>
       <c r="E64" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>102</v>
+        <v>214</v>
       </c>
       <c r="E65" t="s">
         <v>103</v>
@@ -2087,31 +2090,31 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E66" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E67" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E68" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E69" t="s">
         <v>109</v>
@@ -2119,252 +2122,249 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E70" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E71" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C72" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E72" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="C73" t="s">
+        <v>116</v>
+      </c>
       <c r="E73" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E74" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E75" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E76" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E77" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E78" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E79" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E80" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E81" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E82" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E83" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E84" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E85" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E86" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B87" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E87" t="s">
-        <v>208</v>
+        <v>144</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B88" t="s">
         <v>146</v>
       </c>
       <c r="E88" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>145</v>
+        <v>203</v>
       </c>
       <c r="B89" t="s">
         <v>146</v>
       </c>
       <c r="E89" t="s">
-        <v>147</v>
+        <v>204</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>205</v>
+        <v>145</v>
       </c>
       <c r="B90" t="s">
         <v>146</v>
       </c>
       <c r="E90" t="s">
-        <v>204</v>
+        <v>147</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>148</v>
+        <v>205</v>
+      </c>
+      <c r="B91" t="s">
+        <v>146</v>
       </c>
       <c r="E91" t="s">
-        <v>149</v>
+        <v>204</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E92" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E93" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E94" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E95" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E96" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E97" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C98" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E98" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2372,10 +2372,10 @@
         <v>162</v>
       </c>
       <c r="C99" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E99" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2383,10 +2383,10 @@
         <v>162</v>
       </c>
       <c r="C100" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E100" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2394,10 +2394,10 @@
         <v>162</v>
       </c>
       <c r="C101" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E101" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2405,120 +2405,120 @@
         <v>162</v>
       </c>
       <c r="C102" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E102" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="C103" t="s">
+        <v>171</v>
+      </c>
       <c r="E103" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E104" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E105" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E106" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E107" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>218</v>
+        <v>180</v>
       </c>
       <c r="E108" t="s">
-        <v>219</v>
+        <v>181</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>182</v>
+        <v>218</v>
       </c>
       <c r="E109" t="s">
-        <v>183</v>
+        <v>219</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E110" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E111" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B112" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="E112" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B113" t="s">
         <v>146</v>
       </c>
       <c r="E113" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B114" t="s">
         <v>146</v>
       </c>
       <c r="E114" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B115" t="s">
         <v>146</v>
@@ -2528,8 +2528,8 @@
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>202</v>
+      <c r="A116" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="B116" t="s">
         <v>146</v>
@@ -2540,12 +2540,23 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B117" t="s">
         <v>146</v>
       </c>
       <c r="E117" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>206</v>
+      </c>
+      <c r="B118" t="s">
+        <v>146</v>
+      </c>
+      <c r="E118" t="s">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix ILR Permanent Reserve mapping to location facet
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -687,7 +687,7 @@
     <t>Africana Library &gt; A/V</t>
   </si>
   <si>
-    <t xml:space="preserve">ILR Library Permanent Reserve </t>
+    <t xml:space="preserve">ILR Permanent Reserve </t>
   </si>
 </sst>
 </file>
@@ -1532,7 +1532,7 @@
   <dimension ref="A1:E118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add hotel permanent reserve to hierarchical location facet
DISCOVERYACCESS-7433
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="225">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -688,6 +688,12 @@
   </si>
   <si>
     <t xml:space="preserve">ILR Permanent Reserve </t>
+  </si>
+  <si>
+    <t>Nestle Library &gt; Permanent Reserve</t>
+  </si>
+  <si>
+    <t>Nestle Library Permanent Reserve</t>
   </si>
 </sst>
 </file>
@@ -1529,10 +1535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E118"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2138,244 +2144,241 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>113</v>
+        <v>224</v>
       </c>
       <c r="E72" t="s">
-        <v>114</v>
+        <v>223</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C73" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E73" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="C74" t="s">
+        <v>116</v>
+      </c>
       <c r="E74" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E75" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E76" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E77" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E78" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E79" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E80" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E81" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E82" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E83" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E84" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E85" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E86" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E87" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B88" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E88" t="s">
-        <v>208</v>
+        <v>144</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B89" t="s">
         <v>146</v>
       </c>
       <c r="E89" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>145</v>
+        <v>203</v>
       </c>
       <c r="B90" t="s">
         <v>146</v>
       </c>
       <c r="E90" t="s">
-        <v>147</v>
+        <v>204</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>205</v>
+        <v>145</v>
       </c>
       <c r="B91" t="s">
         <v>146</v>
       </c>
       <c r="E91" t="s">
-        <v>204</v>
+        <v>147</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>148</v>
+        <v>205</v>
+      </c>
+      <c r="B92" t="s">
+        <v>146</v>
       </c>
       <c r="E92" t="s">
-        <v>149</v>
+        <v>204</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E93" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E94" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E95" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E96" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E97" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E98" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C99" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E99" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2383,10 +2386,10 @@
         <v>162</v>
       </c>
       <c r="C100" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E100" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2394,10 +2397,10 @@
         <v>162</v>
       </c>
       <c r="C101" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E101" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2405,10 +2408,10 @@
         <v>162</v>
       </c>
       <c r="C102" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E102" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2416,120 +2419,120 @@
         <v>162</v>
       </c>
       <c r="C103" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E103" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="C104" t="s">
+        <v>171</v>
+      </c>
       <c r="E104" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E105" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E106" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E107" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E108" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>218</v>
+        <v>180</v>
       </c>
       <c r="E109" t="s">
-        <v>219</v>
+        <v>181</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>182</v>
+        <v>218</v>
       </c>
       <c r="E110" t="s">
-        <v>183</v>
+        <v>219</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E111" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E112" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B113" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="E113" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B114" t="s">
         <v>146</v>
       </c>
       <c r="E114" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B115" t="s">
         <v>146</v>
       </c>
       <c r="E115" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B116" t="s">
         <v>146</v>
@@ -2539,8 +2542,8 @@
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>202</v>
+      <c r="A117" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="B117" t="s">
         <v>146</v>
@@ -2551,12 +2554,23 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B118" t="s">
         <v>146</v>
       </c>
       <c r="E118" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>206</v>
+      </c>
+      <c r="B119" t="s">
+        <v>146</v>
+      </c>
+      <c r="E119" t="s">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Kheel Center > Request in advance to location facet
DISCOVERYACCESS-8134
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AAC1D45-FF14-4C02-925D-08E8E754B513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27690" windowHeight="8205"/>
+    <workbookView xWindow="2670" yWindow="-14790" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="226">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -694,12 +695,15 @@
   </si>
   <si>
     <t>Nestle Library Permanent Reserve</t>
+  </si>
+  <si>
+    <t>ILR Library Kheel Center &gt; Request in advance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1534,11 +1538,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1810,7 +1814,7 @@
         <v>43</v>
       </c>
       <c r="E31" t="s">
-        <v>41</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add Olin X03 locations to facet mapping
DISCOVERYACCESS-8155
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AAC1D45-FF14-4C02-925D-08E8E754B513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646B97C5-E9DD-4434-8439-6D89FA7EA3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="-14790" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="-13920" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="232">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -698,6 +698,24 @@
   </si>
   <si>
     <t>ILR Library Kheel Center &gt; Request in advance</t>
+  </si>
+  <si>
+    <t>Olin Library Room 603</t>
+  </si>
+  <si>
+    <t>Olin Library &gt; Room 603</t>
+  </si>
+  <si>
+    <t>Olin Library Room 303</t>
+  </si>
+  <si>
+    <t>Olin Library Room 403</t>
+  </si>
+  <si>
+    <t>Olin Library &gt; Room 403</t>
+  </si>
+  <si>
+    <t>Olin Library &gt; Room 303</t>
   </si>
 </sst>
 </file>
@@ -1539,10 +1557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89:XFD89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2287,135 +2305,126 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B89" t="s">
-        <v>146</v>
+        <v>228</v>
       </c>
       <c r="E89" t="s">
-        <v>208</v>
+        <v>231</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B90" t="s">
-        <v>146</v>
+        <v>229</v>
       </c>
       <c r="E90" t="s">
-        <v>204</v>
+        <v>230</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B91" t="s">
-        <v>146</v>
+        <v>226</v>
       </c>
       <c r="E91" t="s">
-        <v>147</v>
+        <v>227</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B92" t="s">
         <v>146</v>
       </c>
       <c r="E92" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>148</v>
+        <v>203</v>
+      </c>
+      <c r="B93" t="s">
+        <v>146</v>
       </c>
       <c r="E93" t="s">
-        <v>149</v>
+        <v>204</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
+      </c>
+      <c r="B94" t="s">
+        <v>146</v>
       </c>
       <c r="E94" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>152</v>
+        <v>205</v>
+      </c>
+      <c r="B95" t="s">
+        <v>146</v>
       </c>
       <c r="E95" t="s">
-        <v>153</v>
+        <v>204</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E96" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="E97" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E98" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E99" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C100" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E100" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C101" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E101" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C102" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E102" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2423,10 +2432,10 @@
         <v>162</v>
       </c>
       <c r="C103" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E103" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2434,147 +2443,180 @@
         <v>162</v>
       </c>
       <c r="C104" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="E104" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="C105" t="s">
+        <v>167</v>
+      </c>
       <c r="E105" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
+      </c>
+      <c r="C106" t="s">
+        <v>169</v>
       </c>
       <c r="E106" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>176</v>
+        <v>162</v>
+      </c>
+      <c r="C107" t="s">
+        <v>171</v>
       </c>
       <c r="E107" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="E108" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E109" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>218</v>
+        <v>176</v>
       </c>
       <c r="E110" t="s">
-        <v>219</v>
+        <v>177</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E111" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E112" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="E113" t="s">
-        <v>187</v>
+        <v>219</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B114" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="E114" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B115" t="s">
-        <v>146</v>
+        <v>184</v>
       </c>
       <c r="E115" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B116" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="E116" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B117" t="s">
         <v>146</v>
       </c>
       <c r="E117" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>202</v>
+      <c r="A118" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="B118" t="s">
         <v>146</v>
       </c>
       <c r="E118" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>206</v>
+      <c r="A119" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="B119" t="s">
         <v>146</v>
       </c>
       <c r="E119" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B120" t="s">
+        <v>146</v>
+      </c>
+      <c r="E120" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>202</v>
+      </c>
+      <c r="B121" t="s">
+        <v>146</v>
+      </c>
+      <c r="E121" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>206</v>
+      </c>
+      <c r="B122" t="s">
+        <v>146</v>
+      </c>
+      <c r="E122" t="s">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Location Facets - Adelson & Africana
DISCOVERYACCESS-8182
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646B97C5-E9DD-4434-8439-6D89FA7EA3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59318806-1319-4F4F-A89A-54FCC36E6CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="-13920" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="630" yWindow="780" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="232">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -31,33 +31,18 @@
     <t>Facet Display Name</t>
   </si>
   <si>
-    <t>Adelson Library (Lab of Ornithology)</t>
-  </si>
-  <si>
     <t>Adelson Library &gt; Main Collection</t>
   </si>
   <si>
-    <t>Adelson Library Reference (Lab of Ornithology)</t>
-  </si>
-  <si>
     <t>Adelson Library &gt; Reference</t>
   </si>
   <si>
-    <t>Museum of Vertebrates (Lab of Ornithology) (non-circulating)</t>
-  </si>
-  <si>
     <t>Adelson Library &gt; Museum of Vertebrates</t>
   </si>
   <si>
-    <t>Macaulay Library (Lab of Ornithology) (Non-circulating)</t>
-  </si>
-  <si>
     <t>Adelson Library &gt; Macaulay Library</t>
   </si>
   <si>
-    <t>Africana Library (Africana Center)</t>
-  </si>
-  <si>
     <t>new book</t>
   </si>
   <si>
@@ -67,15 +52,9 @@
     <t>Africana Library &gt; Main Collection</t>
   </si>
   <si>
-    <t>Africana Library Reference ( Non-Circulating)</t>
-  </si>
-  <si>
     <t>Africana Library &gt; Reference</t>
   </si>
   <si>
-    <t xml:space="preserve">Africana Library Reserve </t>
-  </si>
-  <si>
     <t>Africana Library &gt; Reserve</t>
   </si>
   <si>
@@ -622,12 +601,6 @@
     <t>Mann Library &gt; Ellis Collection</t>
   </si>
   <si>
-    <t>Ornithology Circulation</t>
-  </si>
-  <si>
-    <t>Adelson Library &gt; Circulation</t>
-  </si>
-  <si>
     <t>Clinical Ophthalmology Collection (Departmental use only)</t>
   </si>
   <si>
@@ -682,9 +655,6 @@
     <t>Veterinary Library &gt; Core Textbooks</t>
   </si>
   <si>
-    <t>Africana A/V</t>
-  </si>
-  <si>
     <t>Africana Library &gt; A/V</t>
   </si>
   <si>
@@ -716,6 +686,36 @@
   </si>
   <si>
     <t>Olin Library &gt; Room 303</t>
+  </si>
+  <si>
+    <t>Adelson Library</t>
+  </si>
+  <si>
+    <t>Adelson Library Reference (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Museum of Vertebrates (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Macaulay Library (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Clarke Africana Library A/V</t>
+  </si>
+  <si>
+    <t>Clarke Africana Library New and Noteworthy</t>
+  </si>
+  <si>
+    <t>Clarke Africana Library</t>
+  </si>
+  <si>
+    <t>Clarke Africana Library Permanent Reserve</t>
+  </si>
+  <si>
+    <t>Clarke Africana Library Reference ( Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Clarke Africana Library Reserve</t>
   </si>
 </sst>
 </file>
@@ -1557,10 +1557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89:XFD89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,7 +1574,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1585,10 +1585,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="D2" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -1596,1028 +1596,1036 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E3" t="s">
         <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>224</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>225</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>200</v>
+        <v>226</v>
       </c>
       <c r="E7" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="E8" t="s">
-        <v>221</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>228</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>228</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>230</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>231</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>229</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>213</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="E18" t="s">
-        <v>212</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>202</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>216</v>
+        <v>20</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>208</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E24" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
       </c>
       <c r="E25" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>222</v>
+        <v>26</v>
       </c>
       <c r="E26" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>212</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E29" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E30" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E31" t="s">
-        <v>225</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E32" t="s">
-        <v>45</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E33" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E34" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E35" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E36" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B37" t="s">
-        <v>146</v>
+        <v>44</v>
       </c>
       <c r="E37" t="s">
-        <v>210</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>53</v>
+        <v>200</v>
+      </c>
+      <c r="B38" t="s">
+        <v>139</v>
       </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>201</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E39" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E40" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E41" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E42" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E43" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E44" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E45" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E46" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E47" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E48" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E49" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C50" t="s">
-        <v>198</v>
+        <v>67</v>
       </c>
       <c r="E50" t="s">
-        <v>199</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C51" t="s">
-        <v>77</v>
+        <v>191</v>
       </c>
       <c r="E51" t="s">
-        <v>78</v>
+        <v>192</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
+      </c>
+      <c r="C52" t="s">
+        <v>70</v>
       </c>
       <c r="E52" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="E53" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E54" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E55" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E56" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E57" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>215</v>
+        <v>81</v>
       </c>
       <c r="E58" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>90</v>
+        <v>206</v>
       </c>
       <c r="E59" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E60" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E61" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E62" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E63" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="E64" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>214</v>
+        <v>93</v>
       </c>
       <c r="E65" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>102</v>
+        <v>205</v>
       </c>
       <c r="E66" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E67" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E68" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E69" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E70" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E71" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>224</v>
+        <v>104</v>
       </c>
       <c r="E72" t="s">
-        <v>223</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>113</v>
+        <v>214</v>
       </c>
       <c r="E73" t="s">
-        <v>114</v>
+        <v>213</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C74" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E74" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
+      </c>
+      <c r="C75" t="s">
+        <v>109</v>
       </c>
       <c r="E75" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="E76" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="E77" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="E78" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E79" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E80" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="E81" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E82" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E83" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E84" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E85" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="E86" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E87" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E88" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>228</v>
+        <v>136</v>
       </c>
       <c r="E89" t="s">
-        <v>231</v>
+        <v>137</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="E90" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="E91" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B92" t="s">
-        <v>146</v>
+        <v>216</v>
       </c>
       <c r="E92" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B93" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E93" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>145</v>
+        <v>194</v>
       </c>
       <c r="B94" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E94" t="s">
-        <v>147</v>
+        <v>195</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>205</v>
+        <v>138</v>
       </c>
       <c r="B95" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E95" t="s">
-        <v>204</v>
+        <v>140</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>148</v>
+        <v>196</v>
+      </c>
+      <c r="B96" t="s">
+        <v>139</v>
       </c>
       <c r="E96" t="s">
-        <v>149</v>
+        <v>195</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="E97" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="E98" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="E99" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E100" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E101" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E102" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C103" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E103" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C104" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="E104" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C105" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="E105" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C106" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="E106" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C107" t="s">
         <v>162</v>
       </c>
-      <c r="C107" t="s">
-        <v>171</v>
-      </c>
       <c r="E107" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
+      </c>
+      <c r="C108" t="s">
+        <v>164</v>
       </c>
       <c r="E108" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="E109" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="E110" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="E111" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="E112" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>218</v>
+        <v>173</v>
       </c>
       <c r="E113" t="s">
-        <v>219</v>
+        <v>174</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="E114" t="s">
-        <v>183</v>
+        <v>210</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="E115" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E116" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B117" t="s">
-        <v>146</v>
+        <v>179</v>
       </c>
       <c r="E117" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B118" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E118" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B119" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E119" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B120" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E120" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>202</v>
+      <c r="A121" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="B121" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E121" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="B122" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E122" t="s">
-        <v>193</v>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>197</v>
+      </c>
+      <c r="B123" t="s">
+        <v>139</v>
+      </c>
+      <c r="E123" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Location Facets - CISER & Fine Arts
DISCOVERYACCESS-8182
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59318806-1319-4F4F-A89A-54FCC36E6CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371583A7-2A49-4E96-966A-80E41E9D265A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="780" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1275" yWindow="2790" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="236">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -70,27 +70,12 @@
     <t>Bailey Hortorium &gt; Reference</t>
   </si>
   <si>
-    <t>CISER Data Archive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fine Arts Circulation </t>
-  </si>
-  <si>
-    <t>Fine Arts Library &gt; Circulation</t>
-  </si>
-  <si>
     <t>Fine Arts Library &gt; Main Collection</t>
   </si>
   <si>
-    <t>Fine Arts Library Reference (Non-Circulating)</t>
-  </si>
-  <si>
     <t>Fine Arts Library &gt; Reference</t>
   </si>
   <si>
-    <t>Fine Arts Library Reserve</t>
-  </si>
-  <si>
     <t>Fine Arts Library &gt; Reserve</t>
   </si>
   <si>
@@ -634,21 +619,12 @@
     <t>Fine Arts Library &gt; Artists' Books</t>
   </si>
   <si>
-    <t>Fine Arts Library (Rand Hall)</t>
-  </si>
-  <si>
     <t>Music Library (Lincoln Hall)</t>
   </si>
   <si>
     <t>Mann Special Collections (Request in advance)</t>
   </si>
   <si>
-    <t>Fine Arts Library Permanent Reserve</t>
-  </si>
-  <si>
-    <t>Fine Arts Course Reserve (Ask at Circulation)</t>
-  </si>
-  <si>
     <t>Veterinary Library Core Resource (5 hour loan)</t>
   </si>
   <si>
@@ -716,6 +692,42 @@
   </si>
   <si>
     <t>Clarke Africana Library Reserve</t>
+  </si>
+  <si>
+    <t>Cornell Center for Social Sciences Data Archive</t>
+  </si>
+  <si>
+    <t>CCSS Data Archive</t>
+  </si>
+  <si>
+    <t>Mui Ho Fine Arts Library</t>
+  </si>
+  <si>
+    <t>Mui Ho Fine Arts Library Artists' Books</t>
+  </si>
+  <si>
+    <t>Mui Ho Fine Arts Library Reference (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Fine Arts Library &gt; Permanent Reserve</t>
+  </si>
+  <si>
+    <t>Mui Ho Fine Arts Library Permanent Reserve</t>
+  </si>
+  <si>
+    <t>Mui Ho Fine Arts Library Reserve</t>
+  </si>
+  <si>
+    <t>Mui Ho Fine Arts Library New and Noteworthy</t>
+  </si>
+  <si>
+    <t>Fine Arts Library &gt; New and Noteworthy</t>
+  </si>
+  <si>
+    <t>Mui Ho Fine Arts Library Flats</t>
+  </si>
+  <si>
+    <t>Fine Arts Library &gt; Flats</t>
   </si>
 </sst>
 </file>
@@ -1199,9 +1211,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1557,10 +1568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E123"/>
+  <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1573,54 +1584,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>190</v>
+      <c r="A1" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>222</v>
+      <c r="A3" t="s">
+        <v>214</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>223</v>
+      <c r="A4" t="s">
+        <v>215</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>224</v>
+      <c r="A5" t="s">
+        <v>216</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>225</v>
+      <c r="A6" t="s">
+        <v>217</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -1628,23 +1639,23 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="E7" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>228</v>
+      <c r="A9" t="s">
+        <v>220</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -1654,39 +1665,39 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>228</v>
+      <c r="A10" t="s">
+        <v>220</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>230</v>
+      <c r="A11" t="s">
+        <v>222</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>231</v>
+      <c r="A12" t="s">
+        <v>223</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>229</v>
+      <c r="A13" t="s">
+        <v>221</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="E14" t="s">
@@ -1694,7 +1705,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="E15" t="s">
@@ -1702,930 +1713,938 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
+        <v>224</v>
+      </c>
+      <c r="E16" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E17" t="s">
         <v>16</v>
       </c>
-      <c r="E16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>227</v>
+      </c>
+      <c r="E18" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>228</v>
+      </c>
+      <c r="E20" t="s">
         <v>17</v>
       </c>
-      <c r="E17" t="s">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>230</v>
+      </c>
+      <c r="E21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>231</v>
+      </c>
+      <c r="E22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>232</v>
+      </c>
+      <c r="E23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>234</v>
+      </c>
+      <c r="E24" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>204</v>
       </c>
-      <c r="E18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" t="s">
         <v>20</v>
       </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>195</v>
+      </c>
+      <c r="B39" t="s">
+        <v>134</v>
+      </c>
+      <c r="E39" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="E42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>55</v>
+      </c>
+      <c r="E47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="E48" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>59</v>
+      </c>
+      <c r="E49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>61</v>
+      </c>
+      <c r="E50" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>62</v>
+      </c>
+      <c r="E51" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>64</v>
+      </c>
+      <c r="C52" t="s">
+        <v>186</v>
+      </c>
+      <c r="E52" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" t="s">
+        <v>65</v>
+      </c>
+      <c r="E53" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>64</v>
+      </c>
+      <c r="E54" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>68</v>
+      </c>
+      <c r="E55" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>70</v>
+      </c>
+      <c r="E56" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>72</v>
+      </c>
+      <c r="E57" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>74</v>
+      </c>
+      <c r="E58" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>76</v>
+      </c>
+      <c r="E59" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>200</v>
+      </c>
+      <c r="E60" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>78</v>
+      </c>
+      <c r="E61" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>80</v>
+      </c>
+      <c r="E62" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>82</v>
+      </c>
+      <c r="E63" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>84</v>
+      </c>
+      <c r="E64" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>86</v>
+      </c>
+      <c r="E65" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>88</v>
+      </c>
+      <c r="E66" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>199</v>
+      </c>
+      <c r="E67" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>90</v>
+      </c>
+      <c r="E68" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>92</v>
+      </c>
+      <c r="E69" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>94</v>
+      </c>
+      <c r="E70" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>96</v>
+      </c>
+      <c r="E71" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>98</v>
+      </c>
+      <c r="E72" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>99</v>
+      </c>
+      <c r="E73" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>206</v>
+      </c>
+      <c r="E74" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>101</v>
+      </c>
+      <c r="E75" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>103</v>
+      </c>
+      <c r="C76" t="s">
+        <v>104</v>
+      </c>
+      <c r="E76" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>103</v>
+      </c>
+      <c r="E77" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>107</v>
+      </c>
+      <c r="E78" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>109</v>
+      </c>
+      <c r="E79" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>111</v>
+      </c>
+      <c r="E80" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>113</v>
+      </c>
+      <c r="E81" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>115</v>
+      </c>
+      <c r="E82" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>117</v>
+      </c>
+      <c r="E83" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>119</v>
+      </c>
+      <c r="E84" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>121</v>
+      </c>
+      <c r="E85" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>123</v>
+      </c>
+      <c r="E86" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>125</v>
+      </c>
+      <c r="E87" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>127</v>
+      </c>
+      <c r="E88" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>129</v>
+      </c>
+      <c r="E89" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>131</v>
+      </c>
+      <c r="E90" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>210</v>
+      </c>
+      <c r="E91" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>211</v>
+      </c>
+      <c r="E92" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>208</v>
+      </c>
+      <c r="E93" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>193</v>
+      </c>
+      <c r="B94" t="s">
+        <v>134</v>
+      </c>
+      <c r="E94" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>189</v>
+      </c>
+      <c r="B95" t="s">
+        <v>134</v>
+      </c>
+      <c r="E95" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>133</v>
+      </c>
+      <c r="B96" t="s">
+        <v>134</v>
+      </c>
+      <c r="E96" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>191</v>
+      </c>
+      <c r="B97" t="s">
+        <v>134</v>
+      </c>
+      <c r="E97" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>136</v>
+      </c>
+      <c r="E98" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>138</v>
+      </c>
+      <c r="E99" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>140</v>
+      </c>
+      <c r="E100" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>142</v>
+      </c>
+      <c r="E101" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>144</v>
+      </c>
+      <c r="E102" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>146</v>
+      </c>
+      <c r="E103" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>148</v>
+      </c>
+      <c r="E104" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>150</v>
+      </c>
+      <c r="C105" t="s">
+        <v>151</v>
+      </c>
+      <c r="E105" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>150</v>
+      </c>
+      <c r="C106" t="s">
+        <v>153</v>
+      </c>
+      <c r="E106" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>150</v>
+      </c>
+      <c r="C107" t="s">
+        <v>155</v>
+      </c>
+      <c r="E107" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>150</v>
+      </c>
+      <c r="C108" t="s">
+        <v>157</v>
+      </c>
+      <c r="E108" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>150</v>
+      </c>
+      <c r="C109" t="s">
+        <v>159</v>
+      </c>
+      <c r="E109" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>150</v>
+      </c>
+      <c r="E110" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>162</v>
+      </c>
+      <c r="E111" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>164</v>
+      </c>
+      <c r="E112" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>166</v>
+      </c>
+      <c r="E113" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>168</v>
+      </c>
+      <c r="E114" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>201</v>
+      </c>
+      <c r="E115" t="s">
         <v>202</v>
       </c>
-      <c r="E19" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="E27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E31" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E32" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E34" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E35" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B38" t="s">
-        <v>139</v>
-      </c>
-      <c r="E38" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E39" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E40" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E41" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E42" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E43" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E44" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E45" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E46" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E47" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E48" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E49" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E50" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C51" t="s">
-        <v>191</v>
-      </c>
-      <c r="E51" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C52" t="s">
-        <v>70</v>
-      </c>
-      <c r="E52" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E53" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E54" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E55" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E56" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E57" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E58" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E59" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E60" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E61" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E62" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E63" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E64" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E65" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E66" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E67" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E68" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E69" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E70" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E71" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E72" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E73" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E74" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C75" t="s">
-        <v>109</v>
-      </c>
-      <c r="E75" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E76" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E77" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E78" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E79" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E80" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E81" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E82" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E83" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E84" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E85" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E86" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E87" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>170</v>
+      </c>
+      <c r="E116" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>172</v>
+      </c>
+      <c r="E117" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>174</v>
+      </c>
+      <c r="E118" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>176</v>
+      </c>
+      <c r="B119" t="s">
         <v>134</v>
       </c>
-      <c r="E88" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E89" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E90" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E91" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E92" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B93" t="s">
-        <v>139</v>
-      </c>
-      <c r="E93" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B94" t="s">
-        <v>139</v>
-      </c>
-      <c r="E94" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B95" t="s">
-        <v>139</v>
-      </c>
-      <c r="E95" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B96" t="s">
-        <v>139</v>
-      </c>
-      <c r="E96" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E97" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E98" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E99" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E100" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E101" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E102" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E103" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C104" t="s">
-        <v>156</v>
-      </c>
-      <c r="E104" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C105" t="s">
-        <v>158</v>
-      </c>
-      <c r="E105" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C106" t="s">
-        <v>160</v>
-      </c>
-      <c r="E106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C107" t="s">
-        <v>162</v>
-      </c>
-      <c r="E107" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C108" t="s">
-        <v>164</v>
-      </c>
-      <c r="E108" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E109" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E110" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E111" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E112" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E113" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E114" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E115" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+      <c r="E119" t="s">
         <v>177</v>
       </c>
-      <c r="E116" t="s">
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
+      <c r="B120" t="s">
+        <v>134</v>
+      </c>
+      <c r="E120" t="s">
         <v>179</v>
       </c>
-      <c r="E117" t="s">
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+      <c r="B121" t="s">
+        <v>134</v>
+      </c>
+      <c r="E121" t="s">
         <v>181</v>
-      </c>
-      <c r="B118" t="s">
-        <v>139</v>
-      </c>
-      <c r="E118" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B119" t="s">
-        <v>139</v>
-      </c>
-      <c r="E119" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B120" t="s">
-        <v>139</v>
-      </c>
-      <c r="E120" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B121" t="s">
-        <v>139</v>
-      </c>
-      <c r="E121" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="B122" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E122" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B123" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E123" t="s">
-        <v>186</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>192</v>
+      </c>
+      <c r="B124" t="s">
+        <v>134</v>
+      </c>
+      <c r="E124" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Location Facets - ILR & Kheel
DISCOVERYACCESS-8182
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371583A7-2A49-4E96-966A-80E41E9D265A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27556E5-D628-4913-AB57-DE85623F5900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="2790" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2040" yWindow="840" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="236">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -79,54 +79,9 @@
     <t>Fine Arts Library &gt; Reserve</t>
   </si>
   <si>
-    <t>ILR Library (Ives Hall)</t>
-  </si>
-  <si>
-    <t>ILR Library &gt; Main Collection</t>
-  </si>
-  <si>
-    <t>ILR Library Reference (Non-Circulating)</t>
-  </si>
-  <si>
     <t>Labor Law</t>
   </si>
   <si>
-    <t>ILR Library &gt; Labor Law Reference</t>
-  </si>
-  <si>
-    <t>ILR Library &gt; Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ILR Library Reserve </t>
-  </si>
-  <si>
-    <t>ILR Library &gt; Reserve</t>
-  </si>
-  <si>
-    <t>ILR Multi-Copy Storage</t>
-  </si>
-  <si>
-    <t>ILR Library Kheel Center</t>
-  </si>
-  <si>
-    <t>ILR Library Kheel Center &gt; Main Collection</t>
-  </si>
-  <si>
-    <t>ILR Library Kheel Center (Non-Circulating)</t>
-  </si>
-  <si>
-    <t>ILR Library Kheel Center (Request in advance)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ILR Library Kheel Center Reference </t>
-  </si>
-  <si>
-    <t>ILR Library Kheel Center &gt; Reference</t>
-  </si>
-  <si>
-    <t>ILR Library Kheel Center Reference (Non-Circulating)</t>
-  </si>
-  <si>
     <t>Asia Reserve, Severinghouse Reading Rm., Kroch Library</t>
   </si>
   <si>
@@ -634,18 +589,12 @@
     <t>Africana Library &gt; A/V</t>
   </si>
   <si>
-    <t xml:space="preserve">ILR Permanent Reserve </t>
-  </si>
-  <si>
     <t>Nestle Library &gt; Permanent Reserve</t>
   </si>
   <si>
     <t>Nestle Library Permanent Reserve</t>
   </si>
   <si>
-    <t>ILR Library Kheel Center &gt; Request in advance</t>
-  </si>
-  <si>
     <t>Olin Library Room 603</t>
   </si>
   <si>
@@ -728,6 +677,57 @@
   </si>
   <si>
     <t>Fine Arts Library &gt; Flats</t>
+  </si>
+  <si>
+    <t>Catherwood Library</t>
+  </si>
+  <si>
+    <t>Catherwood Library &gt; Main Collection</t>
+  </si>
+  <si>
+    <t>Catherwood Library Labor Law Reference (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Catherwood Library &gt; Labor Law Reference</t>
+  </si>
+  <si>
+    <t>Catherwood Library Reference (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Catherwood Library &gt; Reference</t>
+  </si>
+  <si>
+    <t>Catherwood Library Multi-Copy Storage</t>
+  </si>
+  <si>
+    <t>Catherwood Library Permanent Reserve</t>
+  </si>
+  <si>
+    <t>Catherwood Library &gt; Reserve</t>
+  </si>
+  <si>
+    <t>Catherwood Library Main Desk</t>
+  </si>
+  <si>
+    <t>Catherwood Library &gt; Main Desk</t>
+  </si>
+  <si>
+    <t>Kheel Center (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Kheel Center &gt; Main Collection</t>
+  </si>
+  <si>
+    <t>Kheel Center (Request in advance)</t>
+  </si>
+  <si>
+    <t>Kheel Center &gt; Request in advance</t>
+  </si>
+  <si>
+    <t>Kheel Center Reference (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Kheel Center &gt; Reference</t>
   </si>
 </sst>
 </file>
@@ -1568,10 +1568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E124"/>
+  <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,7 +1585,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1596,10 +1596,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="D2" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -1631,7 +1631,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -1639,15 +1639,15 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="E7" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -1655,7 +1655,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -1666,7 +1666,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -1674,7 +1674,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1682,7 +1682,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
@@ -1690,7 +1690,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -1714,15 +1714,15 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="E16" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="E17" t="s">
         <v>16</v>
@@ -1730,26 +1730,26 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="E18" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="C19" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="E19" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="E20" t="s">
         <v>17</v>
@@ -1757,15 +1757,15 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="E21" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="E22" t="s">
         <v>18</v>
@@ -1773,878 +1773,870 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="E23" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="E24" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>219</v>
       </c>
       <c r="E25" t="s">
-        <v>20</v>
+        <v>220</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" t="s">
-        <v>22</v>
+        <v>225</v>
       </c>
       <c r="E26" t="s">
-        <v>23</v>
+        <v>220</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>221</v>
       </c>
       <c r="E27" t="s">
-        <v>24</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>204</v>
+        <v>223</v>
+      </c>
+      <c r="C28" t="s">
+        <v>19</v>
       </c>
       <c r="E28" t="s">
-        <v>26</v>
+        <v>222</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>223</v>
       </c>
       <c r="E29" t="s">
-        <v>26</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>226</v>
       </c>
       <c r="E30" t="s">
-        <v>20</v>
+        <v>227</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>228</v>
       </c>
       <c r="E31" t="s">
-        <v>29</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>230</v>
       </c>
       <c r="E32" t="s">
-        <v>29</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="E33" t="s">
-        <v>207</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>234</v>
       </c>
       <c r="E34" t="s">
-        <v>33</v>
+        <v>235</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="E35" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E36" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="E37" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>180</v>
+      </c>
+      <c r="B38" t="s">
+        <v>119</v>
       </c>
       <c r="E38" t="s">
-        <v>40</v>
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>195</v>
-      </c>
-      <c r="B39" t="s">
-        <v>134</v>
+        <v>26</v>
       </c>
       <c r="E39" t="s">
-        <v>196</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="E40" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E41" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E42" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="E43" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="E44" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E45" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E46" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E47" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E48" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E49" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="E50" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>49</v>
+      </c>
+      <c r="C51" t="s">
+        <v>171</v>
       </c>
       <c r="E51" t="s">
-        <v>63</v>
+        <v>172</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C52" t="s">
-        <v>186</v>
+        <v>50</v>
       </c>
       <c r="E52" t="s">
-        <v>187</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>64</v>
-      </c>
-      <c r="C53" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E53" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E54" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E55" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="E56" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E57" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="E58" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>76</v>
+        <v>185</v>
       </c>
       <c r="E59" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>200</v>
+        <v>63</v>
       </c>
       <c r="E60" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="E61" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="E62" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="E63" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="E64" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="E65" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>88</v>
+        <v>184</v>
       </c>
       <c r="E66" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>199</v>
+        <v>75</v>
       </c>
       <c r="E67" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="E68" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="E69" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="E70" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E71" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="E72" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>99</v>
+        <v>190</v>
       </c>
       <c r="E73" t="s">
-        <v>100</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>206</v>
+        <v>86</v>
       </c>
       <c r="E74" t="s">
-        <v>205</v>
+        <v>87</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>101</v>
+        <v>88</v>
+      </c>
+      <c r="C75" t="s">
+        <v>89</v>
       </c>
       <c r="E75" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>103</v>
-      </c>
-      <c r="C76" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="E76" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="E77" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="E78" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="E79" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="E80" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="E81" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="E82" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="E83" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E84" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="E85" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="E86" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="E87" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="E88" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="E89" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>131</v>
+        <v>193</v>
       </c>
       <c r="E90" t="s">
-        <v>132</v>
+        <v>196</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="E91" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="E92" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>208</v>
+        <v>178</v>
+      </c>
+      <c r="B93" t="s">
+        <v>119</v>
       </c>
       <c r="E93" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="B94" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="E94" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>189</v>
+        <v>118</v>
       </c>
       <c r="B95" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="E95" t="s">
-        <v>190</v>
+        <v>120</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>133</v>
+        <v>176</v>
       </c>
       <c r="B96" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="E96" t="s">
-        <v>135</v>
+        <v>175</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>191</v>
-      </c>
-      <c r="B97" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="E97" t="s">
-        <v>190</v>
+        <v>122</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="E98" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="E99" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="E100" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="E101" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="E102" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="E103" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>148</v>
+        <v>135</v>
+      </c>
+      <c r="C104" t="s">
+        <v>136</v>
       </c>
       <c r="E104" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="C105" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E105" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="C106" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E106" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="C107" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="E107" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="C108" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="E108" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>150</v>
-      </c>
-      <c r="C109" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="E109" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E110" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="E111" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="E112" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="E113" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="E114" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>201</v>
+        <v>155</v>
       </c>
       <c r="E115" t="s">
-        <v>202</v>
+        <v>156</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="E116" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="E117" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>174</v>
+        <v>161</v>
+      </c>
+      <c r="B118" t="s">
+        <v>119</v>
       </c>
       <c r="E118" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="B119" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="E119" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="B120" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="E120" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="B121" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="E121" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B122" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="E122" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="B123" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="E123" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>192</v>
-      </c>
-      <c r="B124" t="s">
-        <v>134</v>
-      </c>
-      <c r="E124" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Location Facets - RMC*, Law, Mann, Nestle*, Olin
For RMC and Nestle, withholding top level facet value change for controlled release to limit splitting during deploy.
DISCOVERYACCESS-8182
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27556E5-D628-4913-AB57-DE85623F5900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91259CB9-6FA3-41E0-8188-24836C8751CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="840" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1305" windowWidth="21600" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="215">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -100,36 +100,18 @@
     <t>Kroch Library Asia &gt; Reference</t>
   </si>
   <si>
-    <t>Kroch Library Rare &amp; Manuscripts (Non-Circulating)</t>
-  </si>
-  <si>
     <t>Kroch Library Rare &amp; Manuscripts &gt; Main Collection</t>
   </si>
   <si>
-    <t>Kroch Library Rare &amp; Manuscripts (Request in advance)</t>
-  </si>
-  <si>
     <t>Kroch Library Rare &amp; Manuscripts &gt; Request in Advance</t>
   </si>
   <si>
-    <t>Kroch Library Rare &amp; Manuscripts Reference (Non-Circulating)</t>
-  </si>
-  <si>
     <t>Kroch Library Rare &amp; Manuscripts &gt; Reference</t>
   </si>
   <si>
-    <t>Law Library (Myron Taylor Hall)</t>
-  </si>
-  <si>
     <t>Law Library &gt; Main Collection</t>
   </si>
   <si>
-    <t>Law Library (Myron Taylor Hall) Rare Books</t>
-  </si>
-  <si>
-    <t>Law Library &gt; Rare Books</t>
-  </si>
-  <si>
     <t>Law Library Rare--Request in advance at Law Circulation Desk</t>
   </si>
   <si>
@@ -148,15 +130,9 @@
     <t>Law Library &gt; Reserve</t>
   </si>
   <si>
-    <t xml:space="preserve">Law Library Technical Services </t>
-  </si>
-  <si>
     <t>Law Library &gt; Technical Services</t>
   </si>
   <si>
-    <t>Legal Aid Clinic</t>
-  </si>
-  <si>
     <t>Law Library &gt; Legal Aid Clinic</t>
   </si>
   <si>
@@ -187,12 +163,6 @@
     <t>Mann Library &gt; Collection Development</t>
   </si>
   <si>
-    <t>Mann Library New Book Shelf</t>
-  </si>
-  <si>
-    <t>Mann Library &gt; New Book Shelf</t>
-  </si>
-  <si>
     <t>Mann Library Reference (Non-Circulating)</t>
   </si>
   <si>
@@ -211,30 +181,9 @@
     <t>Mann Library &gt; Special Collections</t>
   </si>
   <si>
-    <t>Mann Serials</t>
-  </si>
-  <si>
-    <t>Mann Library &gt; Serials</t>
-  </si>
-  <si>
-    <t>Mathematics Library (Circulation Desk)</t>
-  </si>
-  <si>
-    <t>Mathematics Library &gt; Circulation Desk</t>
-  </si>
-  <si>
-    <t>Mathematics Library (Malott Hall)</t>
-  </si>
-  <si>
     <t>Mathematics Library &gt; Main Collection</t>
   </si>
   <si>
-    <t>Mathematics Library Locked Press</t>
-  </si>
-  <si>
-    <t>Mathematics Library &gt; Locked Press</t>
-  </si>
-  <si>
     <t>Mathematics Library Reference (Non-Circulating)</t>
   </si>
   <si>
@@ -247,9 +196,6 @@
     <t>Mathematics Library &gt; Reserve</t>
   </si>
   <si>
-    <t>Cox Library of Music (Lincoln Hall)</t>
-  </si>
-  <si>
     <t>Music Library &gt; Main Collection</t>
   </si>
   <si>
@@ -259,54 +205,27 @@
     <t>Music Library &gt; Circulation</t>
   </si>
   <si>
-    <t>Music Library A/V (Non-Circulating)</t>
-  </si>
-  <si>
     <t>Music Library &gt; A/V</t>
   </si>
   <si>
-    <t>Music Library Locked Press (Reference Desk)</t>
-  </si>
-  <si>
     <t>Music Library &gt; Reference</t>
   </si>
   <si>
-    <t xml:space="preserve">Music Library Reference (Non-Circulating) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Music Library Reserve </t>
-  </si>
-  <si>
     <t>Music Library &gt; Reserve</t>
   </si>
   <si>
-    <t xml:space="preserve">Nestle Library Reserve </t>
-  </si>
-  <si>
-    <t>Nestle Library &gt; Reserve</t>
-  </si>
-  <si>
     <t>Olin Library</t>
   </si>
   <si>
     <t>New &amp; Noteworthy</t>
   </si>
   <si>
-    <t>Olin Library &gt; New &amp; Noteworthy Books Shelf</t>
-  </si>
-  <si>
     <t>Olin Library &gt; Main Collection</t>
   </si>
   <si>
-    <t>DCAPS (106G Olin)</t>
-  </si>
-  <si>
     <t>Olin Library &gt; DCAPS (106G Olin)</t>
   </si>
   <si>
-    <t>Map Storage (Request in Advance at Map Room, Olin Library)</t>
-  </si>
-  <si>
     <t>Olin Library &gt; Map Storage</t>
   </si>
   <si>
@@ -316,9 +235,6 @@
     <t>Olin Library &gt; Maps</t>
   </si>
   <si>
-    <t>Olin Library Graduate Study Room 501, Request at Circulation</t>
-  </si>
-  <si>
     <t>Olin Library &gt; Graduate Study Room 501</t>
   </si>
   <si>
@@ -334,69 +250,18 @@
     <t>Olin Library &gt; Reserve</t>
   </si>
   <si>
-    <t>Olin Library Room 301 (Non-Circulating)</t>
-  </si>
-  <si>
-    <t>Olin Library &gt; Room 301</t>
-  </si>
-  <si>
-    <t>Olin Library Room 305 (Non-Circulating)</t>
-  </si>
-  <si>
-    <t>Olin Library &gt; Room 305</t>
-  </si>
-  <si>
-    <t>Olin Library Room 401 (Non-Circulating)</t>
-  </si>
-  <si>
-    <t>Olin Library &gt; Room 401</t>
-  </si>
-  <si>
-    <t>Olin Library Room 404 (Non-Circulating)</t>
-  </si>
-  <si>
-    <t>Olin Library &gt; Room 404</t>
-  </si>
-  <si>
-    <t>Olin Library Room 405 (Non-Circulating)</t>
-  </si>
-  <si>
-    <t>Olin Library &gt; Room 405</t>
-  </si>
-  <si>
-    <t>Olin Library Room 602 (Non-Circulating)</t>
-  </si>
-  <si>
-    <t>Olin Library &gt; Room 602</t>
-  </si>
-  <si>
     <t>Olin Library Room 604-605 (Non-Circulating)</t>
   </si>
   <si>
     <t>Olin Library &gt; Room 604-605</t>
   </si>
   <si>
-    <t>Library Technical Services Review Shelves</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
-    <t>Olin Library &gt; Technical Services Review Shelves</t>
-  </si>
-  <si>
-    <t>Preservation Department (B32 Olin)</t>
-  </si>
-  <si>
     <t>Olin Library &gt; Preservation Department</t>
   </si>
   <si>
-    <t>Request at Olin Circulation Desk</t>
-  </si>
-  <si>
-    <t>Olin Library &gt; Circulation Desk</t>
-  </si>
-  <si>
     <t>Sage Hall Management Library Reference (Non-Circulating)</t>
   </si>
   <si>
@@ -556,12 +421,6 @@
     <t>Networked Resource</t>
   </si>
   <si>
-    <t>OKU Processing</t>
-  </si>
-  <si>
-    <t>Olin Library &gt; OKU Processing</t>
-  </si>
-  <si>
     <t>RMC Technical Services</t>
   </si>
   <si>
@@ -574,12 +433,6 @@
     <t>Fine Arts Library &gt; Artists' Books</t>
   </si>
   <si>
-    <t>Music Library (Lincoln Hall)</t>
-  </si>
-  <si>
-    <t>Mann Special Collections (Request in advance)</t>
-  </si>
-  <si>
     <t>Veterinary Library Core Resource (5 hour loan)</t>
   </si>
   <si>
@@ -589,30 +442,15 @@
     <t>Africana Library &gt; A/V</t>
   </si>
   <si>
-    <t>Nestle Library &gt; Permanent Reserve</t>
-  </si>
-  <si>
-    <t>Nestle Library Permanent Reserve</t>
-  </si>
-  <si>
     <t>Olin Library Room 603</t>
   </si>
   <si>
-    <t>Olin Library &gt; Room 603</t>
-  </si>
-  <si>
     <t>Olin Library Room 303</t>
   </si>
   <si>
     <t>Olin Library Room 403</t>
   </si>
   <si>
-    <t>Olin Library &gt; Room 403</t>
-  </si>
-  <si>
-    <t>Olin Library &gt; Room 303</t>
-  </si>
-  <si>
     <t>Adelson Library</t>
   </si>
   <si>
@@ -728,6 +566,105 @@
   </si>
   <si>
     <t>Kheel Center &gt; Reference</t>
+  </si>
+  <si>
+    <t>Law Library</t>
+  </si>
+  <si>
+    <t>Rare and Manuscript Collections (Request in advance)</t>
+  </si>
+  <si>
+    <t>Rare and Manuscript Collections (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Rare and Manuscript Collections Reference (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Law Library Special Collections (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Law Library &gt; Special Collections</t>
+  </si>
+  <si>
+    <t>Law Library Technical Services (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Law Library Legal Aid Clinic</t>
+  </si>
+  <si>
+    <t>Mann Library Ellis Collection</t>
+  </si>
+  <si>
+    <t>Mann Library New and Noteworthy</t>
+  </si>
+  <si>
+    <t>Mann Library &gt; New and Noteworthy</t>
+  </si>
+  <si>
+    <t>Mathematics Library</t>
+  </si>
+  <si>
+    <t>Mathematics Library Main Desk</t>
+  </si>
+  <si>
+    <t>Mathematics Library &gt; Main Desk</t>
+  </si>
+  <si>
+    <t>Mathematics Library Permanent Reserve</t>
+  </si>
+  <si>
+    <t>Cox Library of Music and Dance</t>
+  </si>
+  <si>
+    <t>Cox Library of Music and Dance A/V (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Cox Library of Music and Dance Locked Press (Reference Desk)</t>
+  </si>
+  <si>
+    <t>Cox Library of Music and Dance Permanent Reserve</t>
+  </si>
+  <si>
+    <t>Cox Library of Music and Dance Reference (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Cox Library of Music and Dance Reserve</t>
+  </si>
+  <si>
+    <t>Music Library &gt; Special Collections</t>
+  </si>
+  <si>
+    <t>Cox Library of Music and Dance Special Collections (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Nestlé Library Reference (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Nestlé Library Main Desk</t>
+  </si>
+  <si>
+    <t>Nestle Library &gt; Main Desk</t>
+  </si>
+  <si>
+    <t>Nestle Library &gt; Reference</t>
+  </si>
+  <si>
+    <t>Olin Library DCAPS</t>
+  </si>
+  <si>
+    <t>Olin Library &gt; New &amp; Noteworthy</t>
+  </si>
+  <si>
+    <t>Olin Library New and Noteworthy</t>
+  </si>
+  <si>
+    <t>Olin Library Map Storage (Request in Advance via olinmaps@cornell.edu)</t>
+  </si>
+  <si>
+    <t>Olin Library Graduate Study Room 501, Request at Circulation Area</t>
+  </si>
+  <si>
+    <t>Olin Library Preservation Department</t>
   </si>
 </sst>
 </file>
@@ -1568,10 +1505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E123"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,7 +1522,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>170</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1596,10 +1533,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>169</v>
+        <v>124</v>
       </c>
       <c r="D2" t="s">
-        <v>168</v>
+        <v>123</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -1607,7 +1544,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>143</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -1615,7 +1552,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>144</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -1623,7 +1560,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>145</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -1631,7 +1568,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>146</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -1639,15 +1576,15 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>147</v>
       </c>
       <c r="E7" t="s">
-        <v>188</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>148</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -1655,7 +1592,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>203</v>
+        <v>149</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -1666,7 +1603,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>203</v>
+        <v>149</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -1674,7 +1611,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>205</v>
+        <v>151</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1682,7 +1619,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>206</v>
+        <v>152</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
@@ -1690,7 +1627,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>204</v>
+        <v>150</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -1714,15 +1651,15 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>207</v>
+        <v>153</v>
       </c>
       <c r="E16" t="s">
-        <v>208</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>209</v>
+        <v>155</v>
       </c>
       <c r="E17" t="s">
         <v>16</v>
@@ -1730,26 +1667,26 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>210</v>
+        <v>156</v>
       </c>
       <c r="E18" t="s">
-        <v>183</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>211</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s">
-        <v>182</v>
+        <v>135</v>
       </c>
       <c r="E19" t="s">
-        <v>183</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>211</v>
+        <v>157</v>
       </c>
       <c r="E20" t="s">
         <v>17</v>
@@ -1757,15 +1694,15 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>213</v>
+        <v>159</v>
       </c>
       <c r="E21" t="s">
-        <v>212</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>214</v>
+        <v>160</v>
       </c>
       <c r="E22" t="s">
         <v>18</v>
@@ -1773,101 +1710,101 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>215</v>
+        <v>161</v>
       </c>
       <c r="E23" t="s">
-        <v>216</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>217</v>
+        <v>163</v>
       </c>
       <c r="E24" t="s">
-        <v>218</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>219</v>
+        <v>165</v>
       </c>
       <c r="E25" t="s">
-        <v>220</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>225</v>
+        <v>171</v>
       </c>
       <c r="E26" t="s">
-        <v>220</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>221</v>
+        <v>167</v>
       </c>
       <c r="E27" t="s">
-        <v>222</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>223</v>
+        <v>169</v>
       </c>
       <c r="C28" t="s">
         <v>19</v>
       </c>
       <c r="E28" t="s">
-        <v>222</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>223</v>
+        <v>169</v>
       </c>
       <c r="E29" t="s">
-        <v>224</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>226</v>
+        <v>172</v>
       </c>
       <c r="E30" t="s">
-        <v>227</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>228</v>
+        <v>174</v>
       </c>
       <c r="E31" t="s">
-        <v>229</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>230</v>
+        <v>176</v>
       </c>
       <c r="E32" t="s">
-        <v>231</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>232</v>
+        <v>178</v>
       </c>
       <c r="E33" t="s">
-        <v>233</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>234</v>
+        <v>180</v>
       </c>
       <c r="E34" t="s">
-        <v>235</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1896,747 +1833,677 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>180</v>
+        <v>133</v>
       </c>
       <c r="B38" t="s">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="E38" t="s">
-        <v>181</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>184</v>
+      </c>
+      <c r="E39" t="s">
         <v>26</v>
-      </c>
-      <c r="E39" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>28</v>
+        <v>183</v>
       </c>
       <c r="E40" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>30</v>
+        <v>185</v>
       </c>
       <c r="E41" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>182</v>
       </c>
       <c r="E42" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>34</v>
+        <v>186</v>
       </c>
       <c r="E43" t="s">
-        <v>35</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E44" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E45" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E46" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>42</v>
+        <v>188</v>
       </c>
       <c r="E47" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>189</v>
       </c>
       <c r="E48" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E49" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E50" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>49</v>
-      </c>
-      <c r="C51" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="E51" t="s">
-        <v>172</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C52" t="s">
-        <v>50</v>
+        <v>126</v>
       </c>
       <c r="E52" t="s">
-        <v>51</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+      <c r="C53" t="s">
+        <v>42</v>
       </c>
       <c r="E53" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E54" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E55" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>191</v>
       </c>
       <c r="E56" t="s">
-        <v>58</v>
+        <v>192</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E57" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E58" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>185</v>
+        <v>51</v>
       </c>
       <c r="E59" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>194</v>
       </c>
       <c r="E60" t="s">
-        <v>64</v>
+        <v>195</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
       <c r="E61" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>196</v>
       </c>
       <c r="E62" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="E63" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="E64" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>73</v>
+        <v>197</v>
       </c>
       <c r="E65" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>184</v>
+        <v>59</v>
       </c>
       <c r="E66" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>75</v>
+        <v>198</v>
       </c>
       <c r="E67" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>77</v>
+        <v>199</v>
       </c>
       <c r="E68" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>201</v>
       </c>
       <c r="E69" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>81</v>
+        <v>200</v>
       </c>
       <c r="E70" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>83</v>
+        <v>202</v>
       </c>
       <c r="E71" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>84</v>
+        <v>204</v>
       </c>
       <c r="E72" t="s">
-        <v>85</v>
+        <v>203</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="E73" t="s">
-        <v>189</v>
+        <v>208</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>86</v>
+        <v>206</v>
       </c>
       <c r="E74" t="s">
-        <v>87</v>
+        <v>207</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>88</v>
-      </c>
-      <c r="C75" t="s">
-        <v>89</v>
+        <v>211</v>
       </c>
       <c r="E75" t="s">
-        <v>90</v>
+        <v>210</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>88</v>
+        <v>64</v>
+      </c>
+      <c r="C76" t="s">
+        <v>65</v>
       </c>
       <c r="E76" t="s">
-        <v>91</v>
+        <v>210</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="E77" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>94</v>
+        <v>209</v>
       </c>
       <c r="E78" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>96</v>
+        <v>212</v>
       </c>
       <c r="E79" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="E80" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="E81" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="E82" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>104</v>
+        <v>213</v>
       </c>
       <c r="E83" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="E84" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="E85" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="E86" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="E87" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>114</v>
+        <v>129</v>
+      </c>
+      <c r="B88" t="s">
+        <v>78</v>
       </c>
       <c r="E88" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>116</v>
+        <v>131</v>
+      </c>
+      <c r="B89" t="s">
+        <v>78</v>
       </c>
       <c r="E89" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>193</v>
+        <v>214</v>
       </c>
       <c r="E90" t="s">
-        <v>196</v>
+        <v>79</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>194</v>
+        <v>80</v>
       </c>
       <c r="E91" t="s">
-        <v>195</v>
+        <v>81</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>191</v>
+        <v>82</v>
       </c>
       <c r="E92" t="s">
-        <v>192</v>
+        <v>83</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>178</v>
-      </c>
-      <c r="B93" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="E93" t="s">
-        <v>179</v>
+        <v>85</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>174</v>
-      </c>
-      <c r="B94" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="E94" t="s">
-        <v>175</v>
+        <v>87</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>118</v>
-      </c>
-      <c r="B95" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="E95" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>176</v>
-      </c>
-      <c r="B96" t="s">
-        <v>119</v>
+        <v>90</v>
+      </c>
+      <c r="C96" t="s">
+        <v>91</v>
       </c>
       <c r="E96" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>121</v>
+        <v>90</v>
+      </c>
+      <c r="C97" t="s">
+        <v>93</v>
       </c>
       <c r="E97" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>123</v>
+        <v>90</v>
+      </c>
+      <c r="C98" t="s">
+        <v>95</v>
       </c>
       <c r="E98" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>125</v>
+        <v>90</v>
+      </c>
+      <c r="C99" t="s">
+        <v>97</v>
       </c>
       <c r="E99" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>127</v>
+        <v>90</v>
+      </c>
+      <c r="C100" t="s">
+        <v>99</v>
       </c>
       <c r="E100" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>129</v>
+        <v>90</v>
       </c>
       <c r="E101" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="E102" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="E103" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>135</v>
-      </c>
-      <c r="C104" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="E104" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>135</v>
-      </c>
-      <c r="C105" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="E105" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>135</v>
-      </c>
-      <c r="C106" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E106" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>135</v>
-      </c>
-      <c r="C107" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="E107" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>135</v>
-      </c>
-      <c r="C108" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="E108" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="E109" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>147</v>
+        <v>116</v>
+      </c>
+      <c r="B110" t="s">
+        <v>78</v>
       </c>
       <c r="E110" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>149</v>
+        <v>118</v>
+      </c>
+      <c r="B111" t="s">
+        <v>78</v>
       </c>
       <c r="E111" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>151</v>
+        <v>120</v>
+      </c>
+      <c r="B112" t="s">
+        <v>78</v>
       </c>
       <c r="E112" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>153</v>
+        <v>122</v>
+      </c>
+      <c r="B113" t="s">
+        <v>78</v>
       </c>
       <c r="E113" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>186</v>
+        <v>128</v>
+      </c>
+      <c r="B114" t="s">
+        <v>78</v>
       </c>
       <c r="E114" t="s">
-        <v>187</v>
+        <v>121</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>155</v>
+        <v>132</v>
+      </c>
+      <c r="B115" t="s">
+        <v>78</v>
       </c>
       <c r="E115" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>157</v>
-      </c>
-      <c r="E116" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>159</v>
-      </c>
-      <c r="E117" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>161</v>
-      </c>
-      <c r="B118" t="s">
-        <v>119</v>
-      </c>
-      <c r="E118" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>163</v>
-      </c>
-      <c r="B119" t="s">
-        <v>119</v>
-      </c>
-      <c r="E119" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>165</v>
-      </c>
-      <c r="B120" t="s">
-        <v>119</v>
-      </c>
-      <c r="E120" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>167</v>
-      </c>
-      <c r="B121" t="s">
-        <v>119</v>
-      </c>
-      <c r="E121" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>173</v>
-      </c>
-      <c r="B122" t="s">
-        <v>119</v>
-      </c>
-      <c r="E122" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>177</v>
-      </c>
-      <c r="B123" t="s">
-        <v>119</v>
-      </c>
-      <c r="E123" t="s">
-        <v>166</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Location Facets - Asia*, Mgmt, Uris, Vet
*Top level facet name change not applied yet for Asia. (Also withholding that for Spacecraft Imaging.
DISCOVERYACCESS-8182
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91259CB9-6FA3-41E0-8188-24836C8751CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240C46F9-BA78-4C04-8B54-229F2E905EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1305" windowWidth="21600" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1890" yWindow="1065" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="208">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -82,21 +82,9 @@
     <t>Labor Law</t>
   </si>
   <si>
-    <t>Asia Reserve, Severinghouse Reading Rm., Kroch Library</t>
-  </si>
-  <si>
-    <t>Kroch Library Asia &gt; Reserve</t>
-  </si>
-  <si>
-    <t>Kroch Library Asia</t>
-  </si>
-  <si>
     <t>Kroch Library Asia &gt; Main Collection</t>
   </si>
   <si>
-    <t>Kroch Library Asia Reference (Non-Circulating)</t>
-  </si>
-  <si>
     <t>Kroch Library Asia &gt; Reference</t>
   </si>
   <si>
@@ -262,18 +250,6 @@
     <t>Olin Library &gt; Preservation Department</t>
   </si>
   <si>
-    <t>Sage Hall Management Library Reference (Non-Circulating)</t>
-  </si>
-  <si>
-    <t>Sage Hall Management Library &gt; Reference</t>
-  </si>
-  <si>
-    <t>Sage Hall Management Library Reserve</t>
-  </si>
-  <si>
-    <t>Sage Hall Management Library &gt; Reserve</t>
-  </si>
-  <si>
     <t>Spacecraft Planetary Imaging Facility (Non-Circulating)</t>
   </si>
   <si>
@@ -286,12 +262,6 @@
     <t>Uris Library &gt; Main Collection</t>
   </si>
   <si>
-    <t>Uris Circulation</t>
-  </si>
-  <si>
-    <t>Uris Library &gt; Circulation</t>
-  </si>
-  <si>
     <t>Uris Library Asia A/V</t>
   </si>
   <si>
@@ -340,15 +310,6 @@
     <t>Uris Library &gt; Reserve</t>
   </si>
   <si>
-    <t xml:space="preserve">Uris Library Reserve Willis Room </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uris Library &gt; Reserve Willis Room </t>
-  </si>
-  <si>
-    <t>Veterinary Library (Schurman Hall)</t>
-  </si>
-  <si>
     <t>Veterinary Library &gt; Main Collection</t>
   </si>
   <si>
@@ -364,33 +325,12 @@
     <t>Veterinary Library &gt; Reference</t>
   </si>
   <si>
-    <t xml:space="preserve">Veterinary Library Reserve </t>
-  </si>
-  <si>
     <t xml:space="preserve">Veterinary Library &gt; Reserve </t>
   </si>
   <si>
-    <t>Anatomic Pathology Collection (Departmental use only)</t>
-  </si>
-  <si>
-    <t>Veterinary Library &gt; Anatomic Pathology Collection</t>
-  </si>
-  <si>
-    <t>Equine Farm Animal Collection (Departmental use only)</t>
-  </si>
-  <si>
-    <t>Veterinary Library &gt; Equine Farm Animal Collection</t>
-  </si>
-  <si>
-    <t>Center for Animal Resources and Education (Dept. use only)</t>
-  </si>
-  <si>
     <t>XXX</t>
   </si>
   <si>
-    <t>Companion Animal Hospital Collection (Departmental use only)</t>
-  </si>
-  <si>
     <t>Holding Note (852$z)</t>
   </si>
   <si>
@@ -406,9 +346,6 @@
     <t>Mann Library &gt; Ellis Collection</t>
   </si>
   <si>
-    <t>Clinical Ophthalmology Collection (Departmental use only)</t>
-  </si>
-  <si>
     <t>Library Tech Services</t>
   </si>
   <si>
@@ -433,9 +370,6 @@
     <t>Fine Arts Library &gt; Artists' Books</t>
   </si>
   <si>
-    <t>Veterinary Library Core Resource (5 hour loan)</t>
-  </si>
-  <si>
     <t>Veterinary Library &gt; Core Textbooks</t>
   </si>
   <si>
@@ -665,6 +599,51 @@
   </si>
   <si>
     <t>Olin Library Preservation Department</t>
+  </si>
+  <si>
+    <t>Kroch Asia Collections</t>
+  </si>
+  <si>
+    <t>Kroch Asia Collections Reference (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Management Library &gt; Reference</t>
+  </si>
+  <si>
+    <t>Management Library &gt; Reserve</t>
+  </si>
+  <si>
+    <t>Management Library Reference (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Management Library Reserve</t>
+  </si>
+  <si>
+    <t>Management Library New and Noteworthy</t>
+  </si>
+  <si>
+    <t>Management Library &gt; New and Noteworthy</t>
+  </si>
+  <si>
+    <t>Uris Library Permanent Reserve</t>
+  </si>
+  <si>
+    <t>Uris Library &gt; Permanent Reserve</t>
+  </si>
+  <si>
+    <t>Uris Library A.D. White Collection</t>
+  </si>
+  <si>
+    <t>Uris Library &gt; A.D. White Library</t>
+  </si>
+  <si>
+    <t>Flower-Sprecher Veterinary Library</t>
+  </si>
+  <si>
+    <t>Flower-Sprecher Veterinary Library Core Resource</t>
+  </si>
+  <si>
+    <t>Flower-Sprecher Veterinary Library Reserve</t>
   </si>
 </sst>
 </file>
@@ -1505,10 +1484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E115"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,7 +1501,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1533,10 +1512,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -1544,7 +1523,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -1552,7 +1531,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -1560,7 +1539,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -1568,7 +1547,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -1576,15 +1555,15 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="E7" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -1592,7 +1571,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -1603,7 +1582,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -1611,7 +1590,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1619,7 +1598,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
@@ -1627,7 +1606,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -1651,15 +1630,15 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="E16" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="E17" t="s">
         <v>16</v>
@@ -1667,26 +1646,26 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="E18" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="C19" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="E19" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="E20" t="s">
         <v>17</v>
@@ -1694,15 +1673,15 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="E21" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="E22" t="s">
         <v>18</v>
@@ -1710,262 +1689,262 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="E23" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="E24" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="E25" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="E26" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="E27" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="C28" t="s">
         <v>19</v>
       </c>
       <c r="E28" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="E29" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="E30" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="E31" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="E32" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="E33" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="E34" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>193</v>
+      </c>
+      <c r="E35" t="s">
         <v>20</v>
-      </c>
-      <c r="E35" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>194</v>
       </c>
       <c r="E36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>112</v>
+      </c>
+      <c r="B37" t="s">
+        <v>74</v>
       </c>
       <c r="E37" t="s">
-        <v>25</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>133</v>
-      </c>
-      <c r="B38" t="s">
-        <v>78</v>
+        <v>162</v>
       </c>
       <c r="E38" t="s">
-        <v>134</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
       <c r="E39" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="E40" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="E41" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="E42" t="s">
-        <v>29</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>186</v>
+        <v>26</v>
       </c>
       <c r="E43" t="s">
-        <v>187</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E44" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E45" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>34</v>
+        <v>166</v>
       </c>
       <c r="E46" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="E47" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>189</v>
+        <v>34</v>
       </c>
       <c r="E48" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E49" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>39</v>
+        <v>168</v>
       </c>
       <c r="E50" t="s">
-        <v>40</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>190</v>
+        <v>37</v>
+      </c>
+      <c r="C51" t="s">
+        <v>106</v>
       </c>
       <c r="E51" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C52" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
       <c r="E52" t="s">
-        <v>127</v>
+        <v>39</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>41</v>
-      </c>
-      <c r="C53" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E53" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1973,239 +1952,239 @@
         <v>41</v>
       </c>
       <c r="E54" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>45</v>
+        <v>169</v>
       </c>
       <c r="E55" t="s">
-        <v>46</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>191</v>
+        <v>43</v>
       </c>
       <c r="E56" t="s">
-        <v>192</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E57" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E58" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>51</v>
+        <v>172</v>
       </c>
       <c r="E59" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="E60" t="s">
-        <v>195</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="E61" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>196</v>
+        <v>50</v>
       </c>
       <c r="E62" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E63" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="E64" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>197</v>
+        <v>55</v>
       </c>
       <c r="E65" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>59</v>
+        <v>176</v>
       </c>
       <c r="E66" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="E67" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="E68" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="E69" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="E70" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="E71" t="s">
-        <v>63</v>
+        <v>181</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="E72" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="E73" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="E74" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>211</v>
+        <v>60</v>
+      </c>
+      <c r="C75" t="s">
+        <v>61</v>
       </c>
       <c r="E75" t="s">
-        <v>210</v>
+        <v>188</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>64</v>
-      </c>
-      <c r="C76" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E76" t="s">
-        <v>210</v>
+        <v>62</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>64</v>
+        <v>187</v>
       </c>
       <c r="E77" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="E78" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>212</v>
+        <v>65</v>
       </c>
       <c r="E79" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>68</v>
+      </c>
+      <c r="E80" t="s">
         <v>69</v>
-      </c>
-      <c r="E80" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E81" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>74</v>
+        <v>191</v>
       </c>
       <c r="E82" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>213</v>
+        <v>119</v>
       </c>
       <c r="E83" t="s">
         <v>71</v>
@@ -2213,297 +2192,242 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="E84" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="E85" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>140</v>
+        <v>72</v>
       </c>
       <c r="E86" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>76</v>
+        <v>108</v>
+      </c>
+      <c r="B87" t="s">
+        <v>74</v>
       </c>
       <c r="E87" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="B88" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E88" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>131</v>
-      </c>
-      <c r="B89" t="s">
-        <v>78</v>
+        <v>192</v>
       </c>
       <c r="E89" t="s">
-        <v>130</v>
+        <v>75</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="E90" t="s">
-        <v>79</v>
+        <v>195</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>80</v>
+        <v>198</v>
       </c>
       <c r="E91" t="s">
-        <v>81</v>
+        <v>196</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>82</v>
+        <v>199</v>
       </c>
       <c r="E92" t="s">
-        <v>83</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E93" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E94" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>88</v>
+        <v>80</v>
+      </c>
+      <c r="C95" t="s">
+        <v>81</v>
       </c>
       <c r="E95" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C96" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E96" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C97" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E97" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C98" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E98" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>80</v>
+      </c>
+      <c r="C99" t="s">
+        <v>89</v>
+      </c>
+      <c r="E99" t="s">
         <v>90</v>
-      </c>
-      <c r="C99" t="s">
-        <v>97</v>
-      </c>
-      <c r="E99" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>90</v>
-      </c>
-      <c r="C100" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="E100" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E101" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>102</v>
+        <v>201</v>
       </c>
       <c r="E102" t="s">
-        <v>103</v>
+        <v>202</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E103" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>106</v>
+        <v>203</v>
       </c>
       <c r="E104" t="s">
-        <v>107</v>
+        <v>204</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>108</v>
+        <v>205</v>
       </c>
       <c r="E105" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>137</v>
+        <v>206</v>
       </c>
       <c r="E106" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="E107" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="E108" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>114</v>
+        <v>207</v>
       </c>
       <c r="E109" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B110" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E110" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>118</v>
-      </c>
-      <c r="B111" t="s">
-        <v>78</v>
-      </c>
-      <c r="E111" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>120</v>
-      </c>
-      <c r="B112" t="s">
-        <v>78</v>
-      </c>
-      <c r="E112" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>122</v>
-      </c>
-      <c r="B113" t="s">
-        <v>78</v>
-      </c>
-      <c r="E113" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>128</v>
-      </c>
-      <c r="B114" t="s">
-        <v>78</v>
-      </c>
-      <c r="E114" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>132</v>
-      </c>
-      <c r="B115" t="s">
-        <v>78</v>
-      </c>
-      <c r="E115" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Location Facets - Nestlé top level facet change
DISCOVERYACCESS-8182
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240C46F9-BA78-4C04-8B54-229F2E905EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D69C565-9C08-436A-9C59-3CCD8810010E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="1065" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2745" yWindow="1935" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -577,12 +577,6 @@
     <t>Nestlé Library Main Desk</t>
   </si>
   <si>
-    <t>Nestle Library &gt; Main Desk</t>
-  </si>
-  <si>
-    <t>Nestle Library &gt; Reference</t>
-  </si>
-  <si>
     <t>Olin Library DCAPS</t>
   </si>
   <si>
@@ -644,6 +638,12 @@
   </si>
   <si>
     <t>Flower-Sprecher Veterinary Library Reserve</t>
+  </si>
+  <si>
+    <t>Nestlé Library &gt; Reference</t>
+  </si>
+  <si>
+    <t>Nestlé Library &gt; Main Desk</t>
   </si>
 </sst>
 </file>
@@ -1486,8 +1486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,7 +1788,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E35" t="s">
         <v>20</v>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E36" t="s">
         <v>21</v>
@@ -2096,7 +2096,7 @@
         <v>183</v>
       </c>
       <c r="E72" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2104,15 +2104,15 @@
         <v>184</v>
       </c>
       <c r="E73" t="s">
-        <v>185</v>
+        <v>207</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E74" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2123,7 +2123,7 @@
         <v>61</v>
       </c>
       <c r="E75" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2136,7 +2136,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E77" t="s">
         <v>63</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E78" t="s">
         <v>64</v>
@@ -2176,7 +2176,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E82" t="s">
         <v>67</v>
@@ -2238,7 +2238,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E89" t="s">
         <v>75</v>
@@ -2246,26 +2246,26 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E90" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E91" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E92" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2357,10 +2357,10 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E102" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2373,15 +2373,15 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E104" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E105" t="s">
         <v>96</v>
@@ -2389,7 +2389,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E106" t="s">
         <v>116</v>
@@ -2413,7 +2413,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E109" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Location Facets - temporarily restore old nestle locs
DISCOVERYACCESS-8182
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D69C565-9C08-436A-9C59-3CCD8810010E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF20423C-94EE-4AC2-92E9-3BF8A679BD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2745" yWindow="1935" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="211">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -640,10 +640,19 @@
     <t>Flower-Sprecher Veterinary Library Reserve</t>
   </si>
   <si>
+    <t>Nestlé Library &gt; Main Desk</t>
+  </si>
+  <si>
     <t>Nestlé Library &gt; Reference</t>
   </si>
   <si>
-    <t>Nestlé Library &gt; Main Desk</t>
+    <t>Nestlé Library &gt; Reserve</t>
+  </si>
+  <si>
+    <t>Nestle Library Reserve</t>
+  </si>
+  <si>
+    <t>Nestle Library Permanent Reserve</t>
   </si>
 </sst>
 </file>
@@ -1484,10 +1493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2096,7 +2105,7 @@
         <v>183</v>
       </c>
       <c r="E72" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2104,87 +2113,87 @@
         <v>184</v>
       </c>
       <c r="E73" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="E74" t="s">
-        <v>186</v>
+        <v>208</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>60</v>
-      </c>
-      <c r="C75" t="s">
-        <v>61</v>
+        <v>209</v>
       </c>
       <c r="E75" t="s">
-        <v>186</v>
+        <v>208</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>60</v>
+        <v>187</v>
       </c>
       <c r="E76" t="s">
-        <v>62</v>
+        <v>186</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>185</v>
+        <v>60</v>
+      </c>
+      <c r="C77" t="s">
+        <v>61</v>
       </c>
       <c r="E77" t="s">
-        <v>63</v>
+        <v>186</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>188</v>
+        <v>60</v>
       </c>
       <c r="E78" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>65</v>
+        <v>185</v>
       </c>
       <c r="E79" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>68</v>
+        <v>188</v>
       </c>
       <c r="E80" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E81" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>189</v>
+        <v>68</v>
       </c>
       <c r="E82" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>119</v>
+        <v>70</v>
       </c>
       <c r="E83" t="s">
         <v>71</v>
@@ -2192,15 +2201,15 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="E84" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E85" t="s">
         <v>71</v>
@@ -2208,102 +2217,96 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="E86" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>108</v>
-      </c>
-      <c r="B87" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="E87" t="s">
-        <v>109</v>
+        <v>71</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>110</v>
-      </c>
-      <c r="B88" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E88" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>190</v>
+        <v>108</v>
+      </c>
+      <c r="B89" t="s">
+        <v>74</v>
       </c>
       <c r="E89" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>195</v>
+        <v>110</v>
+      </c>
+      <c r="B90" t="s">
+        <v>74</v>
       </c>
       <c r="E90" t="s">
-        <v>193</v>
+        <v>109</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E91" t="s">
-        <v>194</v>
+        <v>75</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E92" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>76</v>
+        <v>196</v>
       </c>
       <c r="E93" t="s">
-        <v>77</v>
+        <v>194</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>78</v>
+        <v>197</v>
       </c>
       <c r="E94" t="s">
-        <v>79</v>
+        <v>198</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>80</v>
-      </c>
-      <c r="C95" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E95" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>80</v>
-      </c>
-      <c r="C96" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E96" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2311,10 +2314,10 @@
         <v>80</v>
       </c>
       <c r="C97" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E97" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2322,10 +2325,10 @@
         <v>80</v>
       </c>
       <c r="C98" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E98" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2333,100 +2336,122 @@
         <v>80</v>
       </c>
       <c r="C99" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E99" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>80</v>
       </c>
+      <c r="C100" t="s">
+        <v>87</v>
+      </c>
       <c r="E100" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>92</v>
+        <v>80</v>
+      </c>
+      <c r="C101" t="s">
+        <v>89</v>
       </c>
       <c r="E101" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>199</v>
+        <v>80</v>
       </c>
       <c r="E102" t="s">
-        <v>200</v>
+        <v>91</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E103" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E104" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>203</v>
+        <v>94</v>
       </c>
       <c r="E105" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E106" t="s">
-        <v>116</v>
+        <v>202</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>97</v>
+        <v>203</v>
       </c>
       <c r="E107" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>99</v>
+        <v>204</v>
       </c>
       <c r="E108" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>205</v>
+        <v>97</v>
       </c>
       <c r="E109" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>99</v>
+      </c>
+      <c r="E110" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>205</v>
+      </c>
+      <c r="E111" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>111</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B112" t="s">
         <v>74</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E112" t="s">
         <v>102</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Location Facets - temporarily revert to unaccented Nestle
DISCOVERYACCESS-8182
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF20423C-94EE-4AC2-92E9-3BF8A679BD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19761AAA-E121-4B89-90DE-F8F75D161471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -640,19 +640,19 @@
     <t>Flower-Sprecher Veterinary Library Reserve</t>
   </si>
   <si>
-    <t>Nestlé Library &gt; Main Desk</t>
-  </si>
-  <si>
-    <t>Nestlé Library &gt; Reference</t>
-  </si>
-  <si>
-    <t>Nestlé Library &gt; Reserve</t>
-  </si>
-  <si>
     <t>Nestle Library Reserve</t>
   </si>
   <si>
     <t>Nestle Library Permanent Reserve</t>
+  </si>
+  <si>
+    <t>Nestle Library &gt; Reference</t>
+  </si>
+  <si>
+    <t>Nestle Library &gt; Main Desk</t>
+  </si>
+  <si>
+    <t>Nestle Library &gt; Reserve</t>
   </si>
 </sst>
 </file>
@@ -1496,7 +1496,7 @@
   <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2105,7 +2105,7 @@
         <v>183</v>
       </c>
       <c r="E72" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2113,23 +2113,23 @@
         <v>184</v>
       </c>
       <c r="E73" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>207</v>
+      </c>
+      <c r="E74" t="s">
         <v>210</v>
-      </c>
-      <c r="E74" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E75" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Location Facets - Fix accent on Nestlé
DISCOVERYACCESS-8182
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19761AAA-E121-4B89-90DE-F8F75D161471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E674E5-8B4B-4601-A6C5-EA0DC6E00214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="885" yWindow="-15690" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -646,13 +646,13 @@
     <t>Nestle Library Permanent Reserve</t>
   </si>
   <si>
-    <t>Nestle Library &gt; Reference</t>
-  </si>
-  <si>
-    <t>Nestle Library &gt; Main Desk</t>
-  </si>
-  <si>
-    <t>Nestle Library &gt; Reserve</t>
+    <t>Nestlé Library &gt; Reserve</t>
+  </si>
+  <si>
+    <t>Nestlé Library &gt; Main Desk</t>
+  </si>
+  <si>
+    <t>Nestlé Library &gt; Reference</t>
   </si>
 </sst>
 </file>
@@ -1496,7 +1496,7 @@
   <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2105,7 +2105,7 @@
         <v>183</v>
       </c>
       <c r="E72" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2121,7 +2121,7 @@
         <v>207</v>
       </c>
       <c r="E74" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2129,7 +2129,7 @@
         <v>206</v>
       </c>
       <c r="E75" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Location Facets - Olin x03
Tom confirmed that these are meant to be
Olin Library > Room 303
et al, not
Olin Library > Reserve
as his spreadsheet had suggested.

DISCOVERYACCESS-8182
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E674E5-8B4B-4601-A6C5-EA0DC6E00214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00ACD7DA-DA33-4806-8D58-56B70AA68C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="-15690" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="-14700" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="214">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -653,6 +653,15 @@
   </si>
   <si>
     <t>Nestlé Library &gt; Reference</t>
+  </si>
+  <si>
+    <t>Olin Library &gt; Room 303</t>
+  </si>
+  <si>
+    <t>Olin Library &gt; Room 403</t>
+  </si>
+  <si>
+    <t>Olin Library &gt; Room 603</t>
   </si>
 </sst>
 </file>
@@ -1496,7 +1505,7 @@
   <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2212,7 +2221,7 @@
         <v>119</v>
       </c>
       <c r="E85" t="s">
-        <v>71</v>
+        <v>211</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2220,7 +2229,7 @@
         <v>120</v>
       </c>
       <c r="E86" t="s">
-        <v>71</v>
+        <v>212</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2228,7 +2237,7 @@
         <v>118</v>
       </c>
       <c r="E87" t="s">
-        <v>71</v>
+        <v>213</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Location Facet - Unit library facet changes for Asia, Space
DISCOVERYACCESS-8182
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00ACD7DA-DA33-4806-8D58-56B70AA68C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A3B29C-9103-496C-9603-77164B351132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="-14700" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3570" yWindow="-12705" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -82,12 +82,6 @@
     <t>Labor Law</t>
   </si>
   <si>
-    <t>Kroch Library Asia &gt; Main Collection</t>
-  </si>
-  <si>
-    <t>Kroch Library Asia &gt; Reference</t>
-  </si>
-  <si>
     <t>Kroch Library Rare &amp; Manuscripts &gt; Main Collection</t>
   </si>
   <si>
@@ -253,9 +247,6 @@
     <t>Spacecraft Planetary Imaging Facility (Non-Circulating)</t>
   </si>
   <si>
-    <t>Space Sciences Building</t>
-  </si>
-  <si>
     <t>Uris Library</t>
   </si>
   <si>
@@ -662,6 +653,15 @@
   </si>
   <si>
     <t>Olin Library &gt; Room 603</t>
+  </si>
+  <si>
+    <t>Spacecraft Planetary Imaging</t>
+  </si>
+  <si>
+    <t>Asia Collections &gt; Main Collection</t>
+  </si>
+  <si>
+    <t>Asia Collections &gt; Reference</t>
   </si>
 </sst>
 </file>
@@ -1504,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1519,7 +1519,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1530,10 +1530,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -1541,7 +1541,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -1557,7 +1557,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -1573,15 +1573,15 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -1589,7 +1589,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -1600,7 +1600,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -1608,7 +1608,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -1648,15 +1648,15 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E17" t="s">
         <v>16</v>
@@ -1664,26 +1664,26 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E18" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E19" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E20" t="s">
         <v>17</v>
@@ -1691,15 +1691,15 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E21" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E22" t="s">
         <v>18</v>
@@ -1707,761 +1707,761 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E23" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E24" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E25" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E26" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E27" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C28" t="s">
         <v>19</v>
       </c>
       <c r="E28" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E29" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E30" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E31" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E32" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E33" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E34" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E35" t="s">
-        <v>20</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E36" t="s">
-        <v>21</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E37" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E38" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E39" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E40" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E41" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E42" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E43" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E44" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E45" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E46" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E47" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E48" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E49" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E50" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C51" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E51" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" t="s">
         <v>37</v>
-      </c>
-      <c r="C52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E52" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E53" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E54" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E55" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E56" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E57" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E58" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E59" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E60" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E61" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E62" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E63" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E64" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E65" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E66" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E67" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E68" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E69" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E70" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E71" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E72" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E73" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E74" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E75" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E76" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C77" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E77" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>58</v>
+      </c>
+      <c r="E78" t="s">
         <v>60</v>
-      </c>
-      <c r="E78" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E79" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E80" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E81" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E82" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E83" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E84" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E85" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E86" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E87" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E88" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B89" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E89" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B90" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E90" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E91" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E92" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E93" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E94" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E95" t="s">
-        <v>77</v>
+        <v>211</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E96" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C97" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E97" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>77</v>
+      </c>
+      <c r="C98" t="s">
         <v>80</v>
       </c>
-      <c r="C98" t="s">
-        <v>83</v>
-      </c>
       <c r="E98" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C99" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E99" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C100" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E100" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C101" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E101" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E102" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E103" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E104" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E105" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E106" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E107" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E108" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E109" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E110" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E111" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B112" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E112" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Location Facet - RMC top level change
DISCOVERYACCESS-8182
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franc\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A3B29C-9103-496C-9603-77164B351132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40D29DD-F141-4632-B5CD-E6AECE2BB879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3570" yWindow="-12705" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2025" yWindow="3930" windowWidth="28800" windowHeight="17625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -82,15 +82,6 @@
     <t>Labor Law</t>
   </si>
   <si>
-    <t>Kroch Library Rare &amp; Manuscripts &gt; Main Collection</t>
-  </si>
-  <si>
-    <t>Kroch Library Rare &amp; Manuscripts &gt; Request in Advance</t>
-  </si>
-  <si>
-    <t>Kroch Library Rare &amp; Manuscripts &gt; Reference</t>
-  </si>
-  <si>
     <t>Law Library &gt; Main Collection</t>
   </si>
   <si>
@@ -352,9 +343,6 @@
     <t>RMC Technical Services</t>
   </si>
   <si>
-    <t>Kroch Library Rare &amp; Manuscripts &gt; Technical Services</t>
-  </si>
-  <si>
     <t>Artist</t>
   </si>
   <si>
@@ -662,6 +650,18 @@
   </si>
   <si>
     <t>Asia Collections &gt; Reference</t>
+  </si>
+  <si>
+    <t>Rare &amp; Manuscript &gt; Technical Services</t>
+  </si>
+  <si>
+    <t>Rare &amp; Manuscript &gt; Main Collection</t>
+  </si>
+  <si>
+    <t>Rare &amp; Manuscript &gt; Reference</t>
+  </si>
+  <si>
+    <t>Rare &amp; Manuscript &gt; Request in Advance</t>
   </si>
 </sst>
 </file>
@@ -1505,7 +1505,7 @@
   <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1519,7 +1519,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1530,10 +1530,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -1541,7 +1541,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -1557,7 +1557,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -1573,15 +1573,15 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -1589,7 +1589,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -1600,7 +1600,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -1608,7 +1608,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -1648,15 +1648,15 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E16" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E17" t="s">
         <v>16</v>
@@ -1664,26 +1664,26 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E18" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C19" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E19" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E20" t="s">
         <v>17</v>
@@ -1691,15 +1691,15 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E21" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E22" t="s">
         <v>18</v>
@@ -1707,761 +1707,761 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E24" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E25" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E26" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E27" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C28" t="s">
         <v>19</v>
       </c>
       <c r="E28" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E29" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E30" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E31" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E32" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E33" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E34" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E35" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E36" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E37" t="s">
-        <v>110</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E38" t="s">
-        <v>20</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E39" t="s">
-        <v>21</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E40" t="s">
-        <v>22</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E41" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E42" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E43" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E44" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E45" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E46" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E47" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E48" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E49" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E50" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C51" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E51" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C52" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E52" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>32</v>
+      </c>
+      <c r="E53" t="s">
         <v>35</v>
-      </c>
-      <c r="E53" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E54" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E55" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E56" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E57" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E58" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E59" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E60" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E61" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E62" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E63" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E64" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E65" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E66" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E67" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E68" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E69" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E70" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E71" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E72" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E73" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E74" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E75" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E76" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C77" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E77" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E78" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E79" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E80" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E81" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E82" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E83" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E84" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E85" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E86" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E87" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E88" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B89" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E89" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B90" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E90" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E91" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E92" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E93" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E94" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E95" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E96" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C97" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E97" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>74</v>
+      </c>
+      <c r="C98" t="s">
         <v>77</v>
       </c>
-      <c r="C98" t="s">
-        <v>80</v>
-      </c>
       <c r="E98" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C99" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E99" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C100" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E100" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C101" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E101" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E102" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E103" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E104" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E105" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E106" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E107" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E108" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E109" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E110" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E111" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B112" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E112" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Location Facet - Add law,spres
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franc\Documents\GitHub\da-solr-availability\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40D29DD-F141-4632-B5CD-E6AECE2BB879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2724F35-7A50-46A0-8DF2-E1D54F5F545C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="3930" windowWidth="28800" windowHeight="17625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2505" yWindow="-13440" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="216">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -662,6 +662,12 @@
   </si>
   <si>
     <t>Rare &amp; Manuscript &gt; Request in Advance</t>
+  </si>
+  <si>
+    <t>Law Library Special Reserve</t>
+  </si>
+  <si>
+    <t>Law Library &gt; Special Reserve</t>
   </si>
 </sst>
 </file>
@@ -1502,10 +1508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E112"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1905,42 +1911,39 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>160</v>
+        <v>214</v>
       </c>
       <c r="E47" t="s">
-        <v>28</v>
+        <v>215</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>29</v>
+        <v>160</v>
       </c>
       <c r="E48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E49" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>161</v>
+        <v>30</v>
       </c>
       <c r="E50" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>32</v>
-      </c>
-      <c r="C51" t="s">
-        <v>100</v>
+        <v>161</v>
       </c>
       <c r="E51" t="s">
         <v>101</v>
@@ -1951,87 +1954,90 @@
         <v>32</v>
       </c>
       <c r="C52" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="E52" t="s">
-        <v>34</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>32</v>
       </c>
+      <c r="C53" t="s">
+        <v>33</v>
+      </c>
       <c r="E53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E54" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>162</v>
+        <v>36</v>
       </c>
       <c r="E55" t="s">
-        <v>163</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>38</v>
+        <v>162</v>
       </c>
       <c r="E56" t="s">
-        <v>39</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E57" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E58" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>165</v>
+        <v>42</v>
       </c>
       <c r="E59" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E60" t="s">
-        <v>44</v>
+        <v>166</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E61" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>45</v>
+        <v>167</v>
       </c>
       <c r="E62" t="s">
         <v>46</v>
@@ -2039,47 +2045,47 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E63" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>168</v>
+        <v>47</v>
       </c>
       <c r="E64" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>50</v>
+        <v>168</v>
       </c>
       <c r="E65" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>169</v>
+        <v>50</v>
       </c>
       <c r="E66" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E67" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E68" t="s">
         <v>53</v>
@@ -2087,15 +2093,15 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E69" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E70" t="s">
         <v>54</v>
@@ -2103,39 +2109,39 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E71" t="s">
-        <v>174</v>
+        <v>54</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E72" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E73" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="E74" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E75" t="s">
         <v>201</v>
@@ -2143,18 +2149,15 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="E76" t="s">
-        <v>179</v>
+        <v>201</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>55</v>
-      </c>
-      <c r="C77" t="s">
-        <v>56</v>
+        <v>180</v>
       </c>
       <c r="E77" t="s">
         <v>179</v>
@@ -2164,104 +2167,104 @@
       <c r="A78" t="s">
         <v>55</v>
       </c>
+      <c r="C78" t="s">
+        <v>56</v>
+      </c>
       <c r="E78" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>178</v>
+        <v>55</v>
       </c>
       <c r="E79" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E80" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>60</v>
+        <v>181</v>
       </c>
       <c r="E81" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E82" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E83" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>182</v>
+        <v>65</v>
       </c>
       <c r="E84" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>112</v>
+        <v>182</v>
       </c>
       <c r="E85" t="s">
-        <v>204</v>
+        <v>62</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E86" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E87" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>67</v>
+        <v>111</v>
       </c>
       <c r="E88" t="s">
-        <v>68</v>
+        <v>206</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>102</v>
-      </c>
-      <c r="B89" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E89" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B90" t="s">
         <v>69</v>
@@ -2272,61 +2275,61 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>183</v>
+        <v>104</v>
+      </c>
+      <c r="B91" t="s">
+        <v>69</v>
       </c>
       <c r="E91" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E92" t="s">
-        <v>186</v>
+        <v>70</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E93" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E94" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>71</v>
+        <v>190</v>
       </c>
       <c r="E95" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E96" t="s">
-        <v>73</v>
+        <v>207</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>74</v>
-      </c>
-      <c r="C97" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E97" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2334,10 +2337,10 @@
         <v>74</v>
       </c>
       <c r="C98" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E98" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2345,10 +2348,10 @@
         <v>74</v>
       </c>
       <c r="C99" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E99" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2356,10 +2359,10 @@
         <v>74</v>
       </c>
       <c r="C100" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E100" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2367,100 +2370,111 @@
         <v>74</v>
       </c>
       <c r="C101" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E101" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>74</v>
       </c>
+      <c r="C102" t="s">
+        <v>83</v>
+      </c>
       <c r="E102" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E103" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>192</v>
+        <v>86</v>
       </c>
       <c r="E104" t="s">
-        <v>193</v>
+        <v>87</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>88</v>
+        <v>192</v>
       </c>
       <c r="E105" t="s">
-        <v>89</v>
+        <v>193</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>194</v>
+        <v>88</v>
       </c>
       <c r="E106" t="s">
-        <v>195</v>
+        <v>89</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E107" t="s">
-        <v>90</v>
+        <v>195</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E108" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>91</v>
+        <v>197</v>
       </c>
       <c r="E109" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E110" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>198</v>
+        <v>93</v>
       </c>
       <c r="E111" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>198</v>
+      </c>
+      <c r="E112" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>105</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B113" t="s">
         <v>69</v>
       </c>
-      <c r="E112" t="s">
+      <c r="E113" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Olin CoLab Location
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2724F35-7A50-46A0-8DF2-E1D54F5F545C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BE314F-4BC4-462F-9170-78FFD330B068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="-13440" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="-15060" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="218">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -668,6 +668,12 @@
   </si>
   <si>
     <t>Law Library &gt; Special Reserve</t>
+  </si>
+  <si>
+    <t>Olin Library Digital CoLab</t>
+  </si>
+  <si>
+    <t>Olin Library &gt; Digital CoLab Room 701</t>
   </si>
 </sst>
 </file>
@@ -1508,10 +1514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2264,18 +2270,15 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>102</v>
-      </c>
-      <c r="B90" t="s">
-        <v>69</v>
+        <v>216</v>
       </c>
       <c r="E90" t="s">
-        <v>103</v>
+        <v>217</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B91" t="s">
         <v>69</v>
@@ -2286,61 +2289,61 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>183</v>
+        <v>104</v>
+      </c>
+      <c r="B92" t="s">
+        <v>69</v>
       </c>
       <c r="E92" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E93" t="s">
-        <v>186</v>
+        <v>70</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E94" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E95" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>71</v>
+        <v>190</v>
       </c>
       <c r="E96" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E97" t="s">
-        <v>73</v>
+        <v>207</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>74</v>
-      </c>
-      <c r="C98" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E98" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2348,10 +2351,10 @@
         <v>74</v>
       </c>
       <c r="C99" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E99" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2359,10 +2362,10 @@
         <v>74</v>
       </c>
       <c r="C100" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E100" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2370,10 +2373,10 @@
         <v>74</v>
       </c>
       <c r="C101" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E101" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2381,100 +2384,111 @@
         <v>74</v>
       </c>
       <c r="C102" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E102" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>74</v>
       </c>
+      <c r="C103" t="s">
+        <v>83</v>
+      </c>
       <c r="E103" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E104" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>192</v>
+        <v>86</v>
       </c>
       <c r="E105" t="s">
-        <v>193</v>
+        <v>87</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>88</v>
+        <v>192</v>
       </c>
       <c r="E106" t="s">
-        <v>89</v>
+        <v>193</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>194</v>
+        <v>88</v>
       </c>
       <c r="E107" t="s">
-        <v>195</v>
+        <v>89</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E108" t="s">
-        <v>90</v>
+        <v>195</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E109" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>91</v>
+        <v>197</v>
       </c>
       <c r="E110" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E111" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>198</v>
+        <v>93</v>
       </c>
       <c r="E112" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>198</v>
+      </c>
+      <c r="E113" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>105</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B114" t="s">
         <v>69</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E114" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Catherwood Library Reserve to location facet mapping
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BE314F-4BC4-462F-9170-78FFD330B068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3301DA44-6BA0-429E-9ED7-38E6CF28493A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="-15060" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6375" yWindow="1965" windowWidth="21600" windowHeight="13035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="219">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -674,6 +674,9 @@
   </si>
   <si>
     <t>Olin Library &gt; Digital CoLab Room 701</t>
+  </si>
+  <si>
+    <t>Catherwood Library Reserve</t>
   </si>
 </sst>
 </file>
@@ -1514,10 +1517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,173 +1797,170 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>147</v>
+        <v>218</v>
       </c>
       <c r="E32" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E33" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>184</v>
+        <v>151</v>
       </c>
       <c r="E35" t="s">
-        <v>208</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>106</v>
-      </c>
-      <c r="B37" t="s">
-        <v>69</v>
+        <v>185</v>
       </c>
       <c r="E37" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>155</v>
+        <v>106</v>
+      </c>
+      <c r="B38" t="s">
+        <v>69</v>
       </c>
       <c r="E38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E39" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E40" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E41" t="s">
-        <v>20</v>
+        <v>212</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E42" t="s">
-        <v>158</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>157</v>
       </c>
       <c r="E43" t="s">
-        <v>22</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E44" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E45" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>159</v>
+        <v>25</v>
       </c>
       <c r="E46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>214</v>
+        <v>159</v>
       </c>
       <c r="E47" t="s">
-        <v>215</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>160</v>
+        <v>214</v>
       </c>
       <c r="E48" t="s">
-        <v>28</v>
+        <v>215</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>29</v>
+        <v>160</v>
       </c>
       <c r="E49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E50" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>161</v>
+        <v>30</v>
       </c>
       <c r="E51" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>32</v>
-      </c>
-      <c r="C52" t="s">
-        <v>100</v>
+        <v>161</v>
       </c>
       <c r="E52" t="s">
         <v>101</v>
@@ -1971,87 +1971,90 @@
         <v>32</v>
       </c>
       <c r="C53" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="E53" t="s">
-        <v>34</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>32</v>
       </c>
+      <c r="C54" t="s">
+        <v>33</v>
+      </c>
       <c r="E54" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E55" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>162</v>
+        <v>36</v>
       </c>
       <c r="E56" t="s">
-        <v>163</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>38</v>
+        <v>162</v>
       </c>
       <c r="E57" t="s">
-        <v>39</v>
+        <v>163</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E58" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E59" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>165</v>
+        <v>42</v>
       </c>
       <c r="E60" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E61" t="s">
-        <v>44</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E62" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>45</v>
+        <v>167</v>
       </c>
       <c r="E63" t="s">
         <v>46</v>
@@ -2059,47 +2062,47 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E64" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>168</v>
+        <v>47</v>
       </c>
       <c r="E65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>50</v>
+        <v>168</v>
       </c>
       <c r="E66" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>169</v>
+        <v>50</v>
       </c>
       <c r="E67" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E68" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E69" t="s">
         <v>53</v>
@@ -2107,15 +2110,15 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E70" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E71" t="s">
         <v>54</v>
@@ -2123,39 +2126,39 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E72" t="s">
-        <v>174</v>
+        <v>54</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E73" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E74" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="E75" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E76" t="s">
         <v>201</v>
@@ -2163,18 +2166,15 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="E77" t="s">
-        <v>179</v>
+        <v>201</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>55</v>
-      </c>
-      <c r="C78" t="s">
-        <v>56</v>
+        <v>180</v>
       </c>
       <c r="E78" t="s">
         <v>179</v>
@@ -2184,112 +2184,112 @@
       <c r="A79" t="s">
         <v>55</v>
       </c>
+      <c r="C79" t="s">
+        <v>56</v>
+      </c>
       <c r="E79" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>178</v>
+        <v>55</v>
       </c>
       <c r="E80" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E81" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>60</v>
+        <v>181</v>
       </c>
       <c r="E82" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E83" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E84" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>182</v>
+        <v>65</v>
       </c>
       <c r="E85" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>112</v>
+        <v>182</v>
       </c>
       <c r="E86" t="s">
-        <v>204</v>
+        <v>62</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E87" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E88" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>67</v>
+        <v>111</v>
       </c>
       <c r="E89" t="s">
-        <v>68</v>
+        <v>206</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>216</v>
+        <v>67</v>
       </c>
       <c r="E90" t="s">
-        <v>217</v>
+        <v>68</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>102</v>
-      </c>
-      <c r="B91" t="s">
-        <v>69</v>
+        <v>216</v>
       </c>
       <c r="E91" t="s">
-        <v>103</v>
+        <v>217</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B92" t="s">
         <v>69</v>
@@ -2300,61 +2300,61 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>183</v>
+        <v>104</v>
+      </c>
+      <c r="B93" t="s">
+        <v>69</v>
       </c>
       <c r="E93" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E94" t="s">
-        <v>186</v>
+        <v>70</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E95" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E96" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>71</v>
+        <v>190</v>
       </c>
       <c r="E97" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E98" t="s">
-        <v>73</v>
+        <v>207</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>74</v>
-      </c>
-      <c r="C99" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E99" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2362,10 +2362,10 @@
         <v>74</v>
       </c>
       <c r="C100" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E100" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2373,10 +2373,10 @@
         <v>74</v>
       </c>
       <c r="C101" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E101" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2384,10 +2384,10 @@
         <v>74</v>
       </c>
       <c r="C102" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E102" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2395,104 +2395,116 @@
         <v>74</v>
       </c>
       <c r="C103" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E103" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>74</v>
       </c>
+      <c r="C104" t="s">
+        <v>83</v>
+      </c>
       <c r="E104" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E105" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>192</v>
+        <v>86</v>
       </c>
       <c r="E106" t="s">
-        <v>193</v>
+        <v>87</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>88</v>
+        <v>192</v>
       </c>
       <c r="E107" t="s">
-        <v>89</v>
+        <v>193</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>194</v>
+        <v>88</v>
       </c>
       <c r="E108" t="s">
-        <v>195</v>
+        <v>89</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E109" t="s">
-        <v>90</v>
+        <v>195</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E110" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>91</v>
+        <v>197</v>
       </c>
       <c r="E111" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E112" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>198</v>
+        <v>93</v>
       </c>
       <c r="E113" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>198</v>
+      </c>
+      <c r="E114" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>105</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B115" t="s">
         <v>69</v>
       </c>
-      <c r="E114" t="s">
+      <c r="E115" t="s">
         <v>96</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add olin,resdesk to location facet
Location added: {"code":"olin,resdesk","name":"Olin Library Reserve, Circulation Desk","library":"Olin Library","hoursCode":"olin","id":"c1b0e47a-a9cc-448a-8558-d0a77c74b8ae","primaryServicePoint":"760beccd-362d-45b6-bfae-639565a877f2"}
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3301DA44-6BA0-429E-9ED7-38E6CF28493A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108D77DC-0764-40CB-94B0-8DB30433AC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6375" yWindow="1965" windowWidth="21600" windowHeight="13035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3435" yWindow="-14970" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="220">
   <si>
     <t>Voyager Display Name</t>
   </si>
@@ -677,6 +677,9 @@
   </si>
   <si>
     <t>Catherwood Library Reserve</t>
+  </si>
+  <si>
+    <t>Olin Library Reserve, Circulation Desk</t>
   </si>
 </sst>
 </file>
@@ -1517,10 +1520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E115"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2241,66 +2244,63 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>182</v>
+        <v>219</v>
       </c>
       <c r="E86" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>112</v>
+        <v>182</v>
       </c>
       <c r="E87" t="s">
-        <v>204</v>
+        <v>62</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E88" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E89" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>67</v>
+        <v>111</v>
       </c>
       <c r="E90" t="s">
-        <v>68</v>
+        <v>206</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>216</v>
+        <v>67</v>
       </c>
       <c r="E91" t="s">
-        <v>217</v>
+        <v>68</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>102</v>
-      </c>
-      <c r="B92" t="s">
-        <v>69</v>
+        <v>216</v>
       </c>
       <c r="E92" t="s">
-        <v>103</v>
+        <v>217</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B93" t="s">
         <v>69</v>
@@ -2311,61 +2311,61 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>183</v>
+        <v>104</v>
+      </c>
+      <c r="B94" t="s">
+        <v>69</v>
       </c>
       <c r="E94" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E95" t="s">
-        <v>186</v>
+        <v>70</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E96" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E97" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>71</v>
+        <v>190</v>
       </c>
       <c r="E98" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E99" t="s">
-        <v>73</v>
+        <v>207</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>74</v>
-      </c>
-      <c r="C100" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E100" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2373,10 +2373,10 @@
         <v>74</v>
       </c>
       <c r="C101" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E101" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2384,10 +2384,10 @@
         <v>74</v>
       </c>
       <c r="C102" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E102" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2395,10 +2395,10 @@
         <v>74</v>
       </c>
       <c r="C103" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E103" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2406,100 +2406,111 @@
         <v>74</v>
       </c>
       <c r="C104" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E104" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>74</v>
       </c>
+      <c r="C105" t="s">
+        <v>83</v>
+      </c>
       <c r="E105" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E106" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>192</v>
+        <v>86</v>
       </c>
       <c r="E107" t="s">
-        <v>193</v>
+        <v>87</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>88</v>
+        <v>192</v>
       </c>
       <c r="E108" t="s">
-        <v>89</v>
+        <v>193</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>194</v>
+        <v>88</v>
       </c>
       <c r="E109" t="s">
-        <v>195</v>
+        <v>89</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E110" t="s">
-        <v>90</v>
+        <v>195</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E111" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>91</v>
+        <v>197</v>
       </c>
       <c r="E112" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E113" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>198</v>
+        <v>93</v>
       </c>
       <c r="E114" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>198</v>
+      </c>
+      <c r="E115" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>105</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B116" t="s">
         <v>69</v>
       </c>
-      <c r="E115" t="s">
+      <c r="E116" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change Adelson Library in location facet to Lab of Ornithology
</commit_message>
<xml_diff>
--- a/src/main/resources/LocationFacetMapping.xlsx
+++ b/src/main/resources/LocationFacetMapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbw4\Documents\GitHub\da-solr-availability\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108D77DC-0764-40CB-94B0-8DB30433AC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2BD8B4-E0EA-47A8-990B-1E4EB08FCAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="-14970" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="525" yWindow="-14040" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationFacetMapping" sheetId="1" r:id="rId1"/>
@@ -31,18 +31,6 @@
     <t>Facet Display Name</t>
   </si>
   <si>
-    <t>Adelson Library &gt; Main Collection</t>
-  </si>
-  <si>
-    <t>Adelson Library &gt; Reference</t>
-  </si>
-  <si>
-    <t>Adelson Library &gt; Museum of Vertebrates</t>
-  </si>
-  <si>
-    <t>Adelson Library &gt; Macaulay Library</t>
-  </si>
-  <si>
     <t>new book</t>
   </si>
   <si>
@@ -364,12 +352,6 @@
     <t>Olin Library Room 403</t>
   </si>
   <si>
-    <t>Adelson Library</t>
-  </si>
-  <si>
-    <t>Adelson Library Reference (Non-Circulating)</t>
-  </si>
-  <si>
     <t>Museum of Vertebrates (Non-Circulating)</t>
   </si>
   <si>
@@ -680,6 +662,24 @@
   </si>
   <si>
     <t>Olin Library Reserve, Circulation Desk</t>
+  </si>
+  <si>
+    <t>Lab of Ornithology Reference (Non-Circulating)</t>
+  </si>
+  <si>
+    <t>Lab of Ornithology</t>
+  </si>
+  <si>
+    <t>Lab of Ornithology &gt; Main Collection</t>
+  </si>
+  <si>
+    <t>Lab of Ornithology &gt; Reference</t>
+  </si>
+  <si>
+    <t>Lab of Ornithology &gt; Museum of Vertebrates</t>
+  </si>
+  <si>
+    <t>Lab of Ornithology &gt; Macaulay Library</t>
   </si>
 </sst>
 </file>
@@ -1224,9 +1224,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1264,7 +1264,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1370,7 +1370,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1512,7 +1512,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1522,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1537,7 +1537,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1548,10 +1548,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -1559,959 +1559,959 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>215</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>214</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E16" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E17" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E18" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C19" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E19" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E21" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E22" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E23" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E24" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E25" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E26" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E27" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E29" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E30" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E31" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E32" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E33" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E34" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E35" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E36" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E37" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B38" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E38" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E39" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E40" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="E41" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E42" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E43" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E45" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E46" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E47" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E48" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E49" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E50" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E51" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E52" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C53" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E53" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C54" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E54" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E55" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E56" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="E57" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E58" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E59" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E60" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E61" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E62" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E63" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E64" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E65" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E66" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E67" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E68" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E69" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E70" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="E71" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E72" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E73" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E74" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E75" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E76" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E77" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E78" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C79" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E79" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E80" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E81" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E82" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E83" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E84" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E85" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E86" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="E87" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E88" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E89" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E90" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E91" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E92" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B93" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E93" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B94" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E94" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E95" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E96" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="E97" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E98" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E99" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E100" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C101" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E101" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>70</v>
+      </c>
+      <c r="C102" t="s">
+        <v>73</v>
+      </c>
+      <c r="E102" t="s">
         <v>74</v>
-      </c>
-      <c r="C102" t="s">
-        <v>77</v>
-      </c>
-      <c r="E102" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C103" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E103" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C104" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E104" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C105" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E105" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E106" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E107" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E108" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E109" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E110" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E111" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="E112" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E113" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E114" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E115" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B116" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E116" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>